<commit_message>
fixed barrel radius: 18 -> 24
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AAD138-8CF7-4AC1-990F-54B64D5DBA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208319F7-E637-4679-A0A7-BDF2EB816372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="195">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1217,12 +1217,20 @@
     <t>no</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>capacity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scope: How far a player can see in unit of tiles (tiles are drawn fixed size)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1531,6 +1539,23 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -1760,7 +1785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1998,12 +2023,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2069,65 +2088,80 @@
     <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2924,8 +2958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M93" sqref="M93:N93"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2942,10 +2976,10 @@
       <c r="B1" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="128" t="s">
+      <c r="C1" s="109" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="128"/>
+      <c r="D1" s="109"/>
       <c r="G1" s="56" t="s">
         <v>163</v>
       </c>
@@ -3041,10 +3075,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="115" t="s">
+      <c r="Z2" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="115"/>
+      <c r="AA2" s="118"/>
       <c r="AG2" s="43" t="s">
         <v>86</v>
       </c>
@@ -4962,7 +4996,7 @@
       <c r="B32" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="42"/>
+      <c r="C32" s="132"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
@@ -5290,26 +5324,28 @@
       <c r="B40" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8" t="s">
+      <c r="D40" s="131"/>
+      <c r="E40" s="131"/>
+      <c r="F40" s="131"/>
+      <c r="G40" s="131"/>
+      <c r="H40" s="131"/>
+      <c r="I40" s="131" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="S40" s="112" t="s">
+      <c r="J40" s="131"/>
+      <c r="K40" s="131"/>
+      <c r="L40" s="131"/>
+      <c r="M40" s="128"/>
+      <c r="N40" s="128"/>
+      <c r="O40" s="128"/>
+      <c r="P40" s="128"/>
+      <c r="S40" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="T40" s="112"/>
+      <c r="T40" s="121"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -5319,28 +5355,30 @@
       <c r="B41" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="85" t="s">
+      <c r="C41" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="85" t="s">
+      <c r="D41" s="130"/>
+      <c r="E41" s="130"/>
+      <c r="F41" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="F41" s="86"/>
-      <c r="G41" s="86" t="s">
+      <c r="G41" s="130"/>
+      <c r="H41" s="130"/>
+      <c r="I41" s="130" t="s">
         <v>62</v>
       </c>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
-      <c r="L41" s="86"/>
-      <c r="M41" s="86"/>
-      <c r="N41" s="86"/>
-      <c r="S41" s="112" t="s">
+      <c r="J41" s="130"/>
+      <c r="K41" s="130"/>
+      <c r="L41" s="130"/>
+      <c r="M41" s="129"/>
+      <c r="N41" s="129"/>
+      <c r="O41" s="129"/>
+      <c r="P41" s="129"/>
+      <c r="S41" s="121" t="s">
         <v>77</v>
       </c>
-      <c r="T41" s="112"/>
+      <c r="T41" s="121"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
@@ -5353,28 +5391,30 @@
       <c r="B42" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="85" t="s">
+      <c r="C42" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="85" t="s">
+      <c r="D42" s="130"/>
+      <c r="E42" s="130"/>
+      <c r="F42" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="86"/>
-      <c r="G42" s="86" t="s">
+      <c r="G42" s="130"/>
+      <c r="H42" s="130"/>
+      <c r="I42" s="130" t="s">
         <v>66</v>
       </c>
-      <c r="H42" s="86"/>
-      <c r="I42" s="86"/>
-      <c r="J42" s="86"/>
-      <c r="K42" s="86"/>
-      <c r="L42" s="86"/>
-      <c r="M42" s="86"/>
-      <c r="N42" s="86"/>
-      <c r="S42" s="112" t="s">
+      <c r="J42" s="130"/>
+      <c r="K42" s="130"/>
+      <c r="L42" s="130"/>
+      <c r="M42" s="129"/>
+      <c r="N42" s="129"/>
+      <c r="O42" s="129"/>
+      <c r="P42" s="129"/>
+      <c r="S42" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="T42" s="112"/>
+      <c r="T42" s="121"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -5383,22 +5423,24 @@
     <row r="43" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="127"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127"/>
+      <c r="G43" s="127"/>
+      <c r="H43" s="127"/>
+      <c r="I43" s="127"/>
+      <c r="J43" s="127"/>
+      <c r="K43" s="127"/>
+      <c r="L43" s="127"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
-      <c r="S43" s="112" t="s">
+      <c r="O43" s="129"/>
+      <c r="P43" s="129"/>
+      <c r="S43" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="T43" s="112"/>
+      <c r="T43" s="121"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -5409,18 +5451,20 @@
     <row r="44" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
+      <c r="C44" s="127"/>
+      <c r="D44" s="127"/>
+      <c r="E44" s="127"/>
+      <c r="F44" s="127"/>
+      <c r="G44" s="127"/>
+      <c r="H44" s="127"/>
+      <c r="I44" s="127"/>
+      <c r="J44" s="127"/>
+      <c r="K44" s="127"/>
+      <c r="L44" s="127"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
+      <c r="O44" s="129"/>
+      <c r="P44" s="129"/>
       <c r="S44" s="57"/>
       <c r="T44" s="57"/>
       <c r="U44" s="57"/>
@@ -5429,7 +5473,11 @@
     <row r="46" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="47" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="48" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="49" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="58" t="s">
+        <v>194</v>
+      </c>
+    </row>
     <row r="50" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="51" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C51" s="63" t="s">
@@ -5438,57 +5486,57 @@
       <c r="D51" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="H51" s="118" t="s">
+      <c r="H51" s="123" t="s">
         <v>70</v>
       </c>
-      <c r="I51" s="118"/>
-      <c r="J51" s="118"/>
-      <c r="K51" s="118"/>
-      <c r="L51" s="118"/>
-      <c r="M51" s="118"/>
+      <c r="I51" s="123"/>
+      <c r="J51" s="123"/>
+      <c r="K51" s="123"/>
+      <c r="L51" s="123"/>
+      <c r="M51" s="123"/>
     </row>
     <row r="52" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="93"/>
-      <c r="B52" s="89" t="s">
+      <c r="A52" s="91"/>
+      <c r="B52" s="87" t="s">
         <v>175</v>
       </c>
-      <c r="C52" s="90">
+      <c r="C52" s="88">
         <v>-1</v>
       </c>
-      <c r="D52" s="90">
+      <c r="D52" s="88">
         <v>0</v>
       </c>
-      <c r="E52" s="90">
+      <c r="E52" s="88">
         <v>1</v>
       </c>
-      <c r="F52" s="90">
+      <c r="F52" s="88">
         <v>2</v>
       </c>
-      <c r="G52" s="90">
+      <c r="G52" s="88">
         <v>3</v>
       </c>
-      <c r="H52" s="91">
+      <c r="H52" s="89">
         <v>4</v>
       </c>
-      <c r="I52" s="91">
+      <c r="I52" s="89">
         <v>5</v>
       </c>
-      <c r="J52" s="91">
+      <c r="J52" s="89">
         <v>6</v>
       </c>
-      <c r="K52" s="91">
+      <c r="K52" s="89">
         <v>7</v>
       </c>
-      <c r="L52" s="91">
+      <c r="L52" s="89">
         <v>8</v>
       </c>
-      <c r="M52" s="91">
+      <c r="M52" s="89">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="92"/>
-      <c r="B53" s="92" t="s">
+      <c r="A53" s="90"/>
+      <c r="B53" s="90" t="s">
         <v>71</v>
       </c>
       <c r="C53" s="19">
@@ -5537,8 +5585,8 @@
       </c>
     </row>
     <row r="54" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="92"/>
-      <c r="B54" s="92" t="s">
+      <c r="A54" s="90"/>
+      <c r="B54" s="90" t="s">
         <v>72</v>
       </c>
       <c r="C54" s="51">
@@ -5561,7 +5609,7 @@
         <f t="shared" si="15"/>
         <v>832</v>
       </c>
-      <c r="H54" s="94">
+      <c r="H54" s="92">
         <f t="shared" si="15"/>
         <v>960</v>
       </c>
@@ -5573,7 +5621,7 @@
         <f t="shared" si="15"/>
         <v>1216</v>
       </c>
-      <c r="K54" s="95">
+      <c r="K54" s="93">
         <f t="shared" si="15"/>
         <v>1344</v>
       </c>
@@ -5596,14 +5644,14 @@
       <c r="E55" s="61"/>
       <c r="F55" s="62"/>
       <c r="G55" s="57"/>
-      <c r="H55" s="119" t="s">
+      <c r="H55" s="124" t="s">
         <v>167</v>
       </c>
-      <c r="I55" s="119"/>
-      <c r="J55" s="119"/>
-      <c r="K55" s="119"/>
-      <c r="L55" s="119"/>
-      <c r="M55" s="119"/>
+      <c r="I55" s="124"/>
+      <c r="J55" s="124"/>
+      <c r="K55" s="124"/>
+      <c r="L55" s="124"/>
+      <c r="M55" s="124"/>
     </row>
     <row r="56" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="57" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5655,88 +5703,90 @@
       <c r="I62" t="s">
         <v>98</v>
       </c>
-      <c r="J62" s="126" t="s">
+      <c r="J62" s="112" t="s">
         <v>102</v>
       </c>
-      <c r="K62" s="126"/>
+      <c r="K62" s="112"/>
       <c r="L62" t="s">
         <v>103</v>
       </c>
-      <c r="M62" s="98">
+      <c r="M62" s="96">
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>23</v>
       </c>
-      <c r="O62" s="125" t="s">
+      <c r="O62" s="111" t="s">
         <v>108</v>
       </c>
-      <c r="P62" s="125"/>
-      <c r="Q62" s="125"/>
-      <c r="R62" s="125"/>
-      <c r="S62" s="125"/>
+      <c r="P62" s="111"/>
+      <c r="Q62" s="111"/>
+      <c r="R62" s="111"/>
+      <c r="S62" s="111"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
       <c r="AJ62" s="81"/>
     </row>
     <row r="63" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="93" t="e" vm="25">
+      <c r="A63" s="91" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
-      <c r="B63" s="87" t="s">
+      <c r="B63" s="85" t="s">
         <v>174</v>
       </c>
-      <c r="C63" s="88" t="s">
+      <c r="C63" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="D63" s="88" t="s">
+      <c r="D63" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="E63" s="88" t="s">
+      <c r="E63" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="F63" s="116" t="s">
+      <c r="F63" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="G63" s="116"/>
-      <c r="H63" s="88"/>
-      <c r="I63" s="88" t="s">
+      <c r="G63" s="113"/>
+      <c r="H63" s="86" t="s">
+        <v>193</v>
+      </c>
+      <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="88" t="s">
+      <c r="J63" s="113" t="s">
         <v>99</v>
       </c>
-      <c r="K63" s="88"/>
-      <c r="L63" s="88" t="s">
+      <c r="K63" s="113"/>
+      <c r="L63" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="M63" s="88" t="s">
+      <c r="M63" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="N63" s="88"/>
-      <c r="O63" s="107" t="s">
+      <c r="N63" s="86"/>
+      <c r="O63" s="105" t="s">
         <v>110</v>
       </c>
-      <c r="P63" s="88" t="s">
+      <c r="P63" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="Q63" s="88" t="s">
+      <c r="Q63" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="R63" s="88" t="s">
+      <c r="R63" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="S63" s="108" t="s">
+      <c r="S63" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="T63" s="88"/>
-      <c r="U63" s="116" t="s">
+      <c r="T63" s="86"/>
+      <c r="U63" s="113" t="s">
         <v>119</v>
       </c>
-      <c r="V63" s="116"/>
-      <c r="W63" s="88" t="s">
+      <c r="V63" s="113"/>
+      <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="X63" s="88" t="s">
+      <c r="X63" s="86" t="s">
         <v>121</v>
       </c>
       <c r="Y63" s="57"/>
@@ -5751,64 +5801,66 @@
       <c r="B64" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C64" s="99">
+      <c r="C64" s="97">
         <v>24</v>
       </c>
-      <c r="D64" s="99">
+      <c r="D64" s="97">
         <v>15</v>
       </c>
-      <c r="E64" s="99">
+      <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="117" t="s">
+      <c r="F64" s="122" t="s">
         <v>97</v>
       </c>
-      <c r="G64" s="117"/>
-      <c r="H64" s="99"/>
-      <c r="I64" s="99">
+      <c r="G64" s="122"/>
+      <c r="H64" s="97">
+        <v>1</v>
+      </c>
+      <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="99">
+      <c r="J64" s="117">
         <f t="shared" ref="J64:J69" si="16">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="99"/>
-      <c r="L64" s="99">
+      <c r="K64" s="117"/>
+      <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>11</v>
       </c>
-      <c r="M64" s="99">
+      <c r="M64" s="97">
         <f>21-L64</f>
         <v>10</v>
       </c>
-      <c r="N64" s="99"/>
-      <c r="O64" s="101">
+      <c r="N64" s="97"/>
+      <c r="O64" s="99">
         <f t="shared" ref="O64:O70" si="17">ROUND(D64/health_cap,2)*10</f>
         <v>0.8</v>
       </c>
-      <c r="P64" s="102">
+      <c r="P64" s="100">
         <f t="shared" ref="P64:P70" si="18">ROUND(M64/guns_cap,2)*10</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="Q64" s="103">
+      <c r="Q64" s="101">
         <f t="shared" ref="Q64:Q70" si="19">ROUND(E64/speed_cap,2)*10</f>
         <v>6</v>
       </c>
-      <c r="R64" s="104">
+      <c r="R64" s="102">
         <f t="shared" ref="R64:R70" si="20">ROUND(I64/DPS_cap,2)*10</f>
         <v>0</v>
       </c>
-      <c r="S64" s="105">
+      <c r="S64" s="103">
         <f>SUM(O64:R64)</f>
         <v>10.100000000000001</v>
       </c>
-      <c r="T64" s="99"/>
-      <c r="U64" s="127">
+      <c r="T64" s="97"/>
+      <c r="U64" s="114">
         <f>R64+O64+P64</f>
         <v>4.1000000000000005</v>
       </c>
-      <c r="V64" s="127"/>
-      <c r="W64" s="106" t="s">
+      <c r="V64" s="114"/>
+      <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
       <c r="X64" s="58" t="s">
@@ -5835,19 +5887,21 @@
       <c r="E65" s="54">
         <v>3</v>
       </c>
-      <c r="F65" s="114" t="s">
+      <c r="F65" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="G65" s="114"/>
-      <c r="H65" s="54"/>
+      <c r="G65" s="108"/>
+      <c r="H65" s="54">
+        <v>1</v>
+      </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="54">
+      <c r="J65" s="117">
         <f t="shared" si="16"/>
         <v>32</v>
       </c>
-      <c r="K65" s="54"/>
+      <c r="K65" s="117"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -5878,11 +5932,11 @@
         <v>12.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="124">
+      <c r="U65" s="115">
         <f t="shared" ref="U65:U70" si="23">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="124"/>
+      <c r="V65" s="115"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -5910,19 +5964,21 @@
       <c r="E66" s="54">
         <v>4</v>
       </c>
-      <c r="F66" s="114" t="s">
+      <c r="F66" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="114"/>
-      <c r="H66" s="54"/>
+      <c r="G66" s="108"/>
+      <c r="H66" s="54">
+        <v>1</v>
+      </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="54">
+      <c r="J66" s="117">
         <f t="shared" si="16"/>
         <v>28</v>
       </c>
-      <c r="K66" s="54"/>
+      <c r="K66" s="117"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -5953,11 +6009,11 @@
         <v>14.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="124">
+      <c r="U66" s="115">
         <f t="shared" si="23"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="124"/>
+      <c r="V66" s="115"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -5985,19 +6041,21 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="114" t="s">
+      <c r="F67" s="108" t="s">
         <v>96</v>
       </c>
-      <c r="G67" s="114"/>
-      <c r="H67" s="54"/>
+      <c r="G67" s="108"/>
+      <c r="H67" s="54">
+        <v>1</v>
+      </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="54">
+      <c r="J67" s="117">
         <f t="shared" si="16"/>
         <v>48</v>
       </c>
-      <c r="K67" s="54"/>
+      <c r="K67" s="117"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -6028,11 +6086,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="124">
+      <c r="U67" s="115">
         <f t="shared" si="23"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="124"/>
+      <c r="V67" s="115"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6056,19 +6114,21 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="114" t="s">
+      <c r="F68" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="114"/>
-      <c r="H68" s="54"/>
+      <c r="G68" s="108"/>
+      <c r="H68" s="54">
+        <v>1</v>
+      </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="54">
+      <c r="J68" s="117">
         <f t="shared" si="16"/>
         <v>72</v>
       </c>
-      <c r="K68" s="54"/>
+      <c r="K68" s="117"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -6099,11 +6159,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="124">
+      <c r="U68" s="115">
         <f t="shared" si="23"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="124"/>
+      <c r="V68" s="115"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -6127,19 +6187,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="114" t="s">
+      <c r="F69" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="114"/>
-      <c r="H69" s="54"/>
+      <c r="G69" s="108"/>
+      <c r="H69" s="54">
+        <v>1</v>
+      </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="54">
+      <c r="J69" s="117">
         <f t="shared" si="16"/>
         <v>20</v>
       </c>
-      <c r="K69" s="54"/>
+      <c r="K69" s="117"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -6170,11 +6232,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="124">
+      <c r="U69" s="115">
         <f t="shared" si="23"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="124"/>
+      <c r="V69" s="115"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -6198,19 +6260,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="114" t="s">
+      <c r="F70" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="G70" s="114"/>
-      <c r="H70" s="54"/>
+      <c r="G70" s="108"/>
+      <c r="H70" s="54">
+        <v>1</v>
+      </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="54">
+      <c r="J70" s="117">
         <f t="shared" ref="J70" si="24">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="54"/>
+      <c r="K70" s="117"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -6241,11 +6305,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="124">
+      <c r="U70" s="115">
         <f t="shared" si="23"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="124"/>
+      <c r="V70" s="115"/>
       <c r="W70" s="25" t="s">
         <v>76</v>
       </c>
@@ -6258,52 +6322,52 @@
     <row r="71" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="72" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="73" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="O73" s="115" t="s">
+      <c r="O73" s="118" t="s">
         <v>170</v>
       </c>
-      <c r="P73" s="115"/>
-      <c r="Q73" s="115"/>
-      <c r="R73" s="115"/>
+      <c r="P73" s="118"/>
+      <c r="Q73" s="118"/>
+      <c r="R73" s="118"/>
     </row>
     <row r="74" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="35"/>
       <c r="B74" s="77" t="s">
         <v>131</v>
       </c>
-      <c r="C74" s="109" t="s">
+      <c r="C74" s="107" t="s">
         <v>92</v>
       </c>
-      <c r="D74" s="109" t="s">
+      <c r="D74" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="E74" s="109" t="s">
+      <c r="E74" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="F74" s="120" t="s">
+      <c r="F74" s="110" t="s">
         <v>138</v>
       </c>
-      <c r="G74" s="120"/>
-      <c r="H74" s="120" t="s">
+      <c r="G74" s="110"/>
+      <c r="H74" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="I74" s="120"/>
-      <c r="J74" s="120" t="s">
+      <c r="I74" s="110"/>
+      <c r="J74" s="110" t="s">
         <v>136</v>
       </c>
-      <c r="K74" s="120"/>
-      <c r="L74" s="120"/>
-      <c r="M74" s="120"/>
-      <c r="N74" s="109" t="s">
+      <c r="K74" s="110"/>
+      <c r="L74" s="110"/>
+      <c r="M74" s="110"/>
+      <c r="N74" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="O74" s="120" t="s">
+      <c r="O74" s="110" t="s">
         <v>172</v>
       </c>
-      <c r="P74" s="120"/>
-      <c r="Q74" s="120" t="s">
+      <c r="P74" s="110"/>
+      <c r="Q74" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="R74" s="120"/>
+      <c r="R74" s="110"/>
     </row>
     <row r="75" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="38" t="e" vm="26">
@@ -6316,26 +6380,26 @@
         <v>2</v>
       </c>
       <c r="D75" s="54">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="123" t="s">
+      <c r="F75" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="G75" s="123"/>
-      <c r="H75" s="123">
+      <c r="G75" s="117"/>
+      <c r="H75" s="117">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="123"/>
-      <c r="J75" s="123" t="s">
+      <c r="I75" s="117"/>
+      <c r="J75" s="117" t="s">
         <v>135</v>
       </c>
-      <c r="K75" s="123"/>
-      <c r="L75" s="123"/>
-      <c r="M75" s="123"/>
+      <c r="K75" s="117"/>
+      <c r="L75" s="117"/>
+      <c r="M75" s="117"/>
       <c r="N75" s="78" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
@@ -6346,7 +6410,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="Q75" s="79"/>
-      <c r="R75" s="97"/>
+      <c r="R75" s="95"/>
     </row>
     <row r="76" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="38" t="e" vm="30">
@@ -6364,21 +6428,21 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="123" t="s">
+      <c r="F76" s="117" t="s">
         <v>128</v>
       </c>
-      <c r="G76" s="123"/>
-      <c r="H76" s="123">
+      <c r="G76" s="117"/>
+      <c r="H76" s="117">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="123"/>
-      <c r="J76" s="123" t="s">
+      <c r="I76" s="117"/>
+      <c r="J76" s="117" t="s">
         <v>134</v>
       </c>
-      <c r="K76" s="123"/>
-      <c r="L76" s="123"/>
-      <c r="M76" s="123"/>
+      <c r="K76" s="117"/>
+      <c r="L76" s="117"/>
+      <c r="M76" s="117"/>
       <c r="N76" s="78" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
@@ -6389,7 +6453,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="Q76" s="79"/>
-      <c r="R76" s="97"/>
+      <c r="R76" s="95"/>
     </row>
     <row r="77" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="18"/>
@@ -6397,19 +6461,19 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="111"/>
-      <c r="G77" s="111"/>
-      <c r="H77" s="111"/>
-      <c r="I77" s="111"/>
-      <c r="J77" s="111"/>
-      <c r="K77" s="111"/>
-      <c r="L77" s="111"/>
-      <c r="M77" s="111"/>
-      <c r="N77" s="96"/>
-      <c r="O77" s="110"/>
-      <c r="P77" s="110"/>
-      <c r="Q77" s="110"/>
-      <c r="R77" s="110"/>
+      <c r="F77" s="127"/>
+      <c r="G77" s="127"/>
+      <c r="H77" s="127"/>
+      <c r="I77" s="127"/>
+      <c r="J77" s="127"/>
+      <c r="K77" s="127"/>
+      <c r="L77" s="127"/>
+      <c r="M77" s="127"/>
+      <c r="N77" s="94"/>
+      <c r="O77" s="125"/>
+      <c r="P77" s="125"/>
+      <c r="Q77" s="125"/>
+      <c r="R77" s="125"/>
     </row>
     <row r="78" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="79" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6420,82 +6484,82 @@
       <c r="B80" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="C80" s="109" t="s">
+      <c r="C80" s="107" t="s">
         <v>141</v>
       </c>
-      <c r="D80" s="109" t="s">
+      <c r="D80" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="E80" s="109" t="s">
+      <c r="E80" s="107" t="s">
         <v>147</v>
       </c>
-      <c r="F80" s="120" t="s">
+      <c r="F80" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="G80" s="120"/>
-      <c r="H80" s="120"/>
-      <c r="I80" s="120"/>
-      <c r="J80" s="120"/>
-      <c r="K80" s="120"/>
-      <c r="L80" s="120"/>
-      <c r="M80" s="120"/>
-      <c r="N80" s="120"/>
-      <c r="O80" s="120"/>
-      <c r="P80" s="120"/>
-      <c r="Q80" s="120" t="s">
+      <c r="G80" s="110"/>
+      <c r="H80" s="110"/>
+      <c r="I80" s="110"/>
+      <c r="J80" s="110"/>
+      <c r="K80" s="110"/>
+      <c r="L80" s="110"/>
+      <c r="M80" s="110"/>
+      <c r="N80" s="110"/>
+      <c r="O80" s="110"/>
+      <c r="P80" s="110"/>
+      <c r="Q80" s="110" t="s">
         <v>157</v>
       </c>
-      <c r="R80" s="120"/>
-      <c r="S80" s="120"/>
-      <c r="T80" s="120"/>
-      <c r="U80" s="120"/>
-      <c r="V80" s="120"/>
-      <c r="W80" s="120"/>
-      <c r="X80" s="120"/>
-      <c r="Y80" s="120"/>
-      <c r="Z80" s="120"/>
-      <c r="AA80" s="120"/>
+      <c r="R80" s="110"/>
+      <c r="S80" s="110"/>
+      <c r="T80" s="110"/>
+      <c r="U80" s="110"/>
+      <c r="V80" s="110"/>
+      <c r="W80" s="110"/>
+      <c r="X80" s="110"/>
+      <c r="Y80" s="110"/>
+      <c r="Z80" s="110"/>
+      <c r="AA80" s="110"/>
     </row>
     <row r="81" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="38"/>
       <c r="B81" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="C81" s="100" t="s">
+      <c r="C81" s="98" t="s">
         <v>143</v>
       </c>
       <c r="D81" s="36">
         <v>7</v>
       </c>
-      <c r="E81" s="99">
+      <c r="E81" s="97">
         <v>16</v>
       </c>
-      <c r="F81" s="122" t="s">
+      <c r="F81" s="116" t="s">
         <v>153</v>
       </c>
-      <c r="G81" s="122"/>
-      <c r="H81" s="122"/>
-      <c r="I81" s="122"/>
-      <c r="J81" s="122"/>
-      <c r="K81" s="122"/>
-      <c r="L81" s="122"/>
-      <c r="M81" s="122"/>
-      <c r="N81" s="122"/>
-      <c r="O81" s="122"/>
-      <c r="P81" s="122"/>
-      <c r="Q81" s="122" t="s">
+      <c r="G81" s="116"/>
+      <c r="H81" s="116"/>
+      <c r="I81" s="116"/>
+      <c r="J81" s="116"/>
+      <c r="K81" s="116"/>
+      <c r="L81" s="116"/>
+      <c r="M81" s="116"/>
+      <c r="N81" s="116"/>
+      <c r="O81" s="116"/>
+      <c r="P81" s="116"/>
+      <c r="Q81" s="116" t="s">
         <v>158</v>
       </c>
-      <c r="R81" s="122"/>
-      <c r="S81" s="122"/>
-      <c r="T81" s="122"/>
-      <c r="U81" s="122"/>
-      <c r="V81" s="122"/>
-      <c r="W81" s="122"/>
-      <c r="X81" s="122"/>
-      <c r="Y81" s="122"/>
-      <c r="Z81" s="122"/>
-      <c r="AA81" s="122"/>
+      <c r="R81" s="116"/>
+      <c r="S81" s="116"/>
+      <c r="T81" s="116"/>
+      <c r="U81" s="116"/>
+      <c r="V81" s="116"/>
+      <c r="W81" s="116"/>
+      <c r="X81" s="116"/>
+      <c r="Y81" s="116"/>
+      <c r="Z81" s="116"/>
+      <c r="AA81" s="116"/>
     </row>
     <row r="82" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="38"/>
@@ -6511,30 +6575,30 @@
       <c r="E82" s="54">
         <v>1</v>
       </c>
-      <c r="F82" s="121" t="s">
+      <c r="F82" s="119" t="s">
         <v>155</v>
       </c>
-      <c r="G82" s="121"/>
-      <c r="H82" s="121"/>
-      <c r="I82" s="121"/>
-      <c r="J82" s="121"/>
-      <c r="K82" s="121"/>
-      <c r="L82" s="121"/>
-      <c r="M82" s="121"/>
-      <c r="N82" s="121"/>
-      <c r="O82" s="121"/>
-      <c r="P82" s="121"/>
-      <c r="Q82" s="121"/>
-      <c r="R82" s="121"/>
-      <c r="S82" s="121"/>
-      <c r="T82" s="121"/>
-      <c r="U82" s="121"/>
-      <c r="V82" s="121"/>
-      <c r="W82" s="121"/>
-      <c r="X82" s="121"/>
-      <c r="Y82" s="121"/>
-      <c r="Z82" s="121"/>
-      <c r="AA82" s="121"/>
+      <c r="G82" s="119"/>
+      <c r="H82" s="119"/>
+      <c r="I82" s="119"/>
+      <c r="J82" s="119"/>
+      <c r="K82" s="119"/>
+      <c r="L82" s="119"/>
+      <c r="M82" s="119"/>
+      <c r="N82" s="119"/>
+      <c r="O82" s="119"/>
+      <c r="P82" s="119"/>
+      <c r="Q82" s="119"/>
+      <c r="R82" s="119"/>
+      <c r="S82" s="119"/>
+      <c r="T82" s="119"/>
+      <c r="U82" s="119"/>
+      <c r="V82" s="119"/>
+      <c r="W82" s="119"/>
+      <c r="X82" s="119"/>
+      <c r="Y82" s="119"/>
+      <c r="Z82" s="119"/>
+      <c r="AA82" s="119"/>
     </row>
     <row r="83" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="38"/>
@@ -6550,30 +6614,30 @@
       <c r="E83" s="54">
         <v>1</v>
       </c>
-      <c r="F83" s="121" t="s">
+      <c r="F83" s="119" t="s">
         <v>154</v>
       </c>
-      <c r="G83" s="121"/>
-      <c r="H83" s="121"/>
-      <c r="I83" s="121"/>
-      <c r="J83" s="121"/>
-      <c r="K83" s="121"/>
-      <c r="L83" s="121"/>
-      <c r="M83" s="121"/>
-      <c r="N83" s="121"/>
-      <c r="O83" s="121"/>
-      <c r="P83" s="121"/>
-      <c r="Q83" s="121"/>
-      <c r="R83" s="121"/>
-      <c r="S83" s="121"/>
-      <c r="T83" s="121"/>
-      <c r="U83" s="121"/>
-      <c r="V83" s="121"/>
-      <c r="W83" s="121"/>
-      <c r="X83" s="121"/>
-      <c r="Y83" s="121"/>
-      <c r="Z83" s="121"/>
-      <c r="AA83" s="121"/>
+      <c r="G83" s="119"/>
+      <c r="H83" s="119"/>
+      <c r="I83" s="119"/>
+      <c r="J83" s="119"/>
+      <c r="K83" s="119"/>
+      <c r="L83" s="119"/>
+      <c r="M83" s="119"/>
+      <c r="N83" s="119"/>
+      <c r="O83" s="119"/>
+      <c r="P83" s="119"/>
+      <c r="Q83" s="119"/>
+      <c r="R83" s="119"/>
+      <c r="S83" s="119"/>
+      <c r="T83" s="119"/>
+      <c r="U83" s="119"/>
+      <c r="V83" s="119"/>
+      <c r="W83" s="119"/>
+      <c r="X83" s="119"/>
+      <c r="Y83" s="119"/>
+      <c r="Z83" s="119"/>
+      <c r="AA83" s="119"/>
     </row>
     <row r="84" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="38"/>
@@ -6589,32 +6653,32 @@
       <c r="E84" s="54">
         <v>1</v>
       </c>
-      <c r="F84" s="121" t="s">
+      <c r="F84" s="119" t="s">
         <v>156</v>
       </c>
-      <c r="G84" s="121"/>
-      <c r="H84" s="121"/>
-      <c r="I84" s="121"/>
-      <c r="J84" s="121"/>
-      <c r="K84" s="121"/>
-      <c r="L84" s="121"/>
-      <c r="M84" s="121"/>
-      <c r="N84" s="121"/>
-      <c r="O84" s="121"/>
-      <c r="P84" s="121"/>
-      <c r="Q84" s="121" t="s">
+      <c r="G84" s="119"/>
+      <c r="H84" s="119"/>
+      <c r="I84" s="119"/>
+      <c r="J84" s="119"/>
+      <c r="K84" s="119"/>
+      <c r="L84" s="119"/>
+      <c r="M84" s="119"/>
+      <c r="N84" s="119"/>
+      <c r="O84" s="119"/>
+      <c r="P84" s="119"/>
+      <c r="Q84" s="119" t="s">
         <v>159</v>
       </c>
-      <c r="R84" s="121"/>
-      <c r="S84" s="121"/>
-      <c r="T84" s="121"/>
-      <c r="U84" s="121"/>
-      <c r="V84" s="121"/>
-      <c r="W84" s="121"/>
-      <c r="X84" s="121"/>
-      <c r="Y84" s="121"/>
-      <c r="Z84" s="121"/>
-      <c r="AA84" s="121"/>
+      <c r="R84" s="119"/>
+      <c r="S84" s="119"/>
+      <c r="T84" s="119"/>
+      <c r="U84" s="119"/>
+      <c r="V84" s="119"/>
+      <c r="W84" s="119"/>
+      <c r="X84" s="119"/>
+      <c r="Y84" s="119"/>
+      <c r="Z84" s="119"/>
+      <c r="AA84" s="119"/>
     </row>
     <row r="85" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="38"/>
@@ -6622,28 +6686,28 @@
       <c r="C85" s="65"/>
       <c r="D85" s="54"/>
       <c r="E85" s="54"/>
-      <c r="F85" s="121"/>
-      <c r="G85" s="121"/>
-      <c r="H85" s="121"/>
-      <c r="I85" s="121"/>
-      <c r="J85" s="121"/>
-      <c r="K85" s="121"/>
-      <c r="L85" s="121"/>
-      <c r="M85" s="121"/>
-      <c r="N85" s="121"/>
-      <c r="O85" s="121"/>
-      <c r="P85" s="121"/>
-      <c r="Q85" s="121"/>
-      <c r="R85" s="121"/>
-      <c r="S85" s="121"/>
-      <c r="T85" s="121"/>
-      <c r="U85" s="121"/>
-      <c r="V85" s="121"/>
-      <c r="W85" s="121"/>
-      <c r="X85" s="121"/>
-      <c r="Y85" s="121"/>
-      <c r="Z85" s="121"/>
-      <c r="AA85" s="121"/>
+      <c r="F85" s="119"/>
+      <c r="G85" s="119"/>
+      <c r="H85" s="119"/>
+      <c r="I85" s="119"/>
+      <c r="J85" s="119"/>
+      <c r="K85" s="119"/>
+      <c r="L85" s="119"/>
+      <c r="M85" s="119"/>
+      <c r="N85" s="119"/>
+      <c r="O85" s="119"/>
+      <c r="P85" s="119"/>
+      <c r="Q85" s="119"/>
+      <c r="R85" s="119"/>
+      <c r="S85" s="119"/>
+      <c r="T85" s="119"/>
+      <c r="U85" s="119"/>
+      <c r="V85" s="119"/>
+      <c r="W85" s="119"/>
+      <c r="X85" s="119"/>
+      <c r="Y85" s="119"/>
+      <c r="Z85" s="119"/>
+      <c r="AA85" s="119"/>
     </row>
     <row r="86" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="38"/>
@@ -6651,28 +6715,28 @@
       <c r="C86" s="65"/>
       <c r="D86" s="54"/>
       <c r="E86" s="54"/>
-      <c r="F86" s="121"/>
-      <c r="G86" s="121"/>
-      <c r="H86" s="121"/>
-      <c r="I86" s="121"/>
-      <c r="J86" s="121"/>
-      <c r="K86" s="121"/>
-      <c r="L86" s="121"/>
-      <c r="M86" s="121"/>
-      <c r="N86" s="121"/>
-      <c r="O86" s="121"/>
-      <c r="P86" s="121"/>
-      <c r="Q86" s="121"/>
-      <c r="R86" s="121"/>
-      <c r="S86" s="121"/>
-      <c r="T86" s="121"/>
-      <c r="U86" s="121"/>
-      <c r="V86" s="121"/>
-      <c r="W86" s="121"/>
-      <c r="X86" s="121"/>
-      <c r="Y86" s="121"/>
-      <c r="Z86" s="121"/>
-      <c r="AA86" s="121"/>
+      <c r="F86" s="119"/>
+      <c r="G86" s="119"/>
+      <c r="H86" s="119"/>
+      <c r="I86" s="119"/>
+      <c r="J86" s="119"/>
+      <c r="K86" s="119"/>
+      <c r="L86" s="119"/>
+      <c r="M86" s="119"/>
+      <c r="N86" s="119"/>
+      <c r="O86" s="119"/>
+      <c r="P86" s="119"/>
+      <c r="Q86" s="119"/>
+      <c r="R86" s="119"/>
+      <c r="S86" s="119"/>
+      <c r="T86" s="119"/>
+      <c r="U86" s="119"/>
+      <c r="V86" s="119"/>
+      <c r="W86" s="119"/>
+      <c r="X86" s="119"/>
+      <c r="Y86" s="119"/>
+      <c r="Z86" s="119"/>
+      <c r="AA86" s="119"/>
     </row>
     <row r="87" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="88" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6681,25 +6745,25 @@
       <c r="B89" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="C89" s="113" t="s">
+      <c r="C89" s="126" t="s">
         <v>182</v>
       </c>
-      <c r="D89" s="113"/>
-      <c r="E89" s="113"/>
-      <c r="F89" s="113"/>
-      <c r="G89" s="113"/>
-      <c r="H89" s="113" t="s">
+      <c r="D89" s="126"/>
+      <c r="E89" s="126"/>
+      <c r="F89" s="126"/>
+      <c r="G89" s="126"/>
+      <c r="H89" s="126" t="s">
         <v>142</v>
       </c>
-      <c r="I89" s="113"/>
-      <c r="J89" s="113"/>
-      <c r="K89" s="113"/>
-      <c r="L89" s="113"/>
-      <c r="M89" s="120" t="s">
+      <c r="I89" s="126"/>
+      <c r="J89" s="126"/>
+      <c r="K89" s="126"/>
+      <c r="L89" s="126"/>
+      <c r="M89" s="110" t="s">
         <v>191</v>
       </c>
-      <c r="N89" s="120"/>
-      <c r="O89" s="109"/>
+      <c r="N89" s="110"/>
+      <c r="O89" s="107"/>
     </row>
     <row r="90" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="38" t="e" vm="35">
@@ -6708,24 +6772,24 @@
       <c r="B90" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C90" s="129" t="s">
+      <c r="C90" s="120" t="s">
         <v>185</v>
       </c>
-      <c r="D90" s="129"/>
-      <c r="E90" s="129"/>
-      <c r="F90" s="129"/>
-      <c r="G90" s="129"/>
-      <c r="H90" s="129" t="s">
+      <c r="D90" s="120"/>
+      <c r="E90" s="120"/>
+      <c r="F90" s="120"/>
+      <c r="G90" s="120"/>
+      <c r="H90" s="120" t="s">
         <v>187</v>
       </c>
-      <c r="I90" s="129"/>
-      <c r="J90" s="129"/>
-      <c r="K90" s="129"/>
-      <c r="L90" s="129"/>
-      <c r="M90" s="114" t="s">
+      <c r="I90" s="120"/>
+      <c r="J90" s="120"/>
+      <c r="K90" s="120"/>
+      <c r="L90" s="120"/>
+      <c r="M90" s="108" t="s">
         <v>192</v>
       </c>
-      <c r="N90" s="114"/>
+      <c r="N90" s="108"/>
       <c r="O90" s="65"/>
     </row>
     <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -6735,24 +6799,24 @@
       <c r="B91" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="C91" s="129" t="s">
+      <c r="C91" s="120" t="s">
         <v>188</v>
       </c>
-      <c r="D91" s="129"/>
-      <c r="E91" s="129"/>
-      <c r="F91" s="129"/>
-      <c r="G91" s="129"/>
-      <c r="H91" s="129" t="s">
+      <c r="D91" s="120"/>
+      <c r="E91" s="120"/>
+      <c r="F91" s="120"/>
+      <c r="G91" s="120"/>
+      <c r="H91" s="120" t="s">
         <v>190</v>
       </c>
-      <c r="I91" s="129"/>
-      <c r="J91" s="129"/>
-      <c r="K91" s="129"/>
-      <c r="L91" s="129"/>
-      <c r="M91" s="114" t="s">
+      <c r="I91" s="120"/>
+      <c r="J91" s="120"/>
+      <c r="K91" s="120"/>
+      <c r="L91" s="120"/>
+      <c r="M91" s="108" t="s">
         <v>192</v>
       </c>
-      <c r="N91" s="114"/>
+      <c r="N91" s="108"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -6762,146 +6826,96 @@
       <c r="B92" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="C92" s="129" t="s">
+      <c r="C92" s="120" t="s">
         <v>189</v>
       </c>
-      <c r="D92" s="129"/>
-      <c r="E92" s="129"/>
-      <c r="F92" s="129"/>
-      <c r="G92" s="129"/>
-      <c r="H92" s="129" t="s">
+      <c r="D92" s="120"/>
+      <c r="E92" s="120"/>
+      <c r="F92" s="120"/>
+      <c r="G92" s="120"/>
+      <c r="H92" s="120" t="s">
         <v>186</v>
       </c>
-      <c r="I92" s="129"/>
-      <c r="J92" s="129"/>
-      <c r="K92" s="129"/>
-      <c r="L92" s="129"/>
-      <c r="M92" s="114" t="s">
+      <c r="I92" s="120"/>
+      <c r="J92" s="120"/>
+      <c r="K92" s="120"/>
+      <c r="L92" s="120"/>
+      <c r="M92" s="108" t="s">
         <v>192</v>
       </c>
-      <c r="N92" s="114"/>
+      <c r="N92" s="108"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="38"/>
       <c r="B93" s="38"/>
-      <c r="C93" s="129"/>
-      <c r="D93" s="129"/>
-      <c r="E93" s="129"/>
-      <c r="F93" s="129"/>
-      <c r="G93" s="129"/>
-      <c r="H93" s="129"/>
-      <c r="I93" s="129"/>
-      <c r="J93" s="129"/>
-      <c r="K93" s="129"/>
-      <c r="L93" s="129"/>
-      <c r="M93" s="114"/>
-      <c r="N93" s="114"/>
+      <c r="C93" s="120"/>
+      <c r="D93" s="120"/>
+      <c r="E93" s="120"/>
+      <c r="F93" s="120"/>
+      <c r="G93" s="120"/>
+      <c r="H93" s="120"/>
+      <c r="I93" s="120"/>
+      <c r="J93" s="120"/>
+      <c r="K93" s="120"/>
+      <c r="L93" s="120"/>
+      <c r="M93" s="108"/>
+      <c r="N93" s="108"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="38"/>
       <c r="B94" s="38"/>
-      <c r="C94" s="129"/>
-      <c r="D94" s="129"/>
-      <c r="E94" s="129"/>
-      <c r="F94" s="129"/>
-      <c r="G94" s="129"/>
-      <c r="H94" s="129"/>
-      <c r="I94" s="129"/>
-      <c r="J94" s="129"/>
-      <c r="K94" s="129"/>
-      <c r="L94" s="129"/>
-      <c r="M94" s="114"/>
-      <c r="N94" s="114"/>
+      <c r="C94" s="120"/>
+      <c r="D94" s="120"/>
+      <c r="E94" s="120"/>
+      <c r="F94" s="120"/>
+      <c r="G94" s="120"/>
+      <c r="H94" s="120"/>
+      <c r="I94" s="120"/>
+      <c r="J94" s="120"/>
+      <c r="K94" s="120"/>
+      <c r="L94" s="120"/>
+      <c r="M94" s="108"/>
+      <c r="N94" s="108"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="38"/>
       <c r="B95" s="38"/>
-      <c r="C95" s="129"/>
-      <c r="D95" s="129"/>
-      <c r="E95" s="129"/>
-      <c r="F95" s="129"/>
-      <c r="G95" s="129"/>
-      <c r="H95" s="129"/>
-      <c r="I95" s="129"/>
-      <c r="J95" s="129"/>
-      <c r="K95" s="129"/>
-      <c r="L95" s="129"/>
-      <c r="M95" s="114"/>
-      <c r="N95" s="114"/>
+      <c r="C95" s="120"/>
+      <c r="D95" s="120"/>
+      <c r="E95" s="120"/>
+      <c r="F95" s="120"/>
+      <c r="G95" s="120"/>
+      <c r="H95" s="120"/>
+      <c r="I95" s="120"/>
+      <c r="J95" s="120"/>
+      <c r="K95" s="120"/>
+      <c r="L95" s="120"/>
+      <c r="M95" s="108"/>
+      <c r="N95" s="108"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="97" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="98" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="78">
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M89:N89"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="F80:P80"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q80:AA80"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H51:M51"/>
-    <mergeCell ref="H55:M55"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C94:G94"/>
+  <mergeCells count="100">
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
     <mergeCell ref="C95:G95"/>
     <mergeCell ref="S42:T42"/>
     <mergeCell ref="S41:T41"/>
@@ -6916,6 +6930,78 @@
     <mergeCell ref="F77:G77"/>
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="J77:M77"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H51:M51"/>
+    <mergeCell ref="H55:M55"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q80:AA80"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="F80:P80"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M89:N89"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nerfed ak47 reload speed
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208319F7-E637-4679-A0A7-BDF2EB816372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DE6EDB-9BD3-4504-B2EE-423BD15E4A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="37">
+  <futureMetadata name="XLRICHVALUE" count="39">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -313,8 +313,22 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="37"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="38"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="37">
+  <valueMetadata count="39">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -425,13 +439,19 @@
     </bk>
     <bk>
       <rc t="1" v="36"/>
+    </bk>
+    <bk>
+      <rc t="1" v="37"/>
+    </bk>
+    <bk>
+      <rc t="1" v="38"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="203">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1223,6 +1243,38 @@
   </si>
   <si>
     <t>Scope: How far a player can see in unit of tiles (tiles are drawn fixed size)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consumable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Restrictions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heal amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>medkit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bandage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 (max)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player health must be blow 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Game objective: not decided yet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1785,7 +1837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2088,80 +2140,84 @@
     <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2230,13 +2286,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>488966</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>6366</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2274,13 +2330,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>488966</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>6366</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2318,13 +2374,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>488966</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>6366</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2362,13 +2418,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>488966</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>6366</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2446,6 +2502,274 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>260350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="타원 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{005E130F-836E-A5DE-A8F0-D0099A88FECF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="24053800"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>260350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="타원 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1D1782A-C202-488E-827F-8761B1624A48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="24053800"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>260350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="타원 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5D39FAC-627D-4745-820C-52C2A6EB616F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="24053800"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>260350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="타원 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F71F03F-8B8E-4306-9792-26CF5D292912}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="24053800"/>
+          <a:ext cx="215900" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2490,7 +2814,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="37">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="39">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -2639,6 +2963,14 @@
     <v>36</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>37</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>38</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -2690,6 +3022,8 @@
   <rel r:id="rId35"/>
   <rel r:id="rId36"/>
   <rel r:id="rId37"/>
+  <rel r:id="rId38"/>
+  <rel r:id="rId39"/>
 </richValueRels>
 </file>
 
@@ -2958,8 +3292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2976,10 +3310,10 @@
       <c r="B1" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="131" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="109"/>
+      <c r="D1" s="131"/>
       <c r="G1" s="56" t="s">
         <v>163</v>
       </c>
@@ -3075,10 +3409,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="118" t="s">
+      <c r="Z2" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="118"/>
+      <c r="AA2" s="121"/>
       <c r="AG2" s="43" t="s">
         <v>86</v>
       </c>
@@ -4216,7 +4550,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="19">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K19" s="19">
         <v>5</v>
@@ -4228,7 +4562,7 @@
       </c>
       <c r="N19" s="19">
         <f>ROUND(E19*F19/(G19+J19)*1000,2)</f>
-        <v>0.9</v>
+        <v>0.47</v>
       </c>
       <c r="O19" s="19">
         <f>E19*F19*I19</f>
@@ -4996,7 +5330,7 @@
       <c r="B32" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="132"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
@@ -5281,33 +5615,7 @@
       <c r="X37" s="74"/>
       <c r="Y37" s="74"/>
     </row>
-    <row r="38" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="74"/>
-      <c r="T38" s="74"/>
-      <c r="U38" s="74"/>
-      <c r="V38" s="74"/>
-      <c r="W38" s="74"/>
-      <c r="X38" s="74"/>
-      <c r="Y38" s="74"/>
-    </row>
+    <row r="38" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="39" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="36"/>
       <c r="B39" s="36"/>
@@ -5324,28 +5632,28 @@
       <c r="B40" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="C40" s="131" t="s">
+      <c r="C40" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="131"/>
-      <c r="E40" s="131"/>
-      <c r="F40" s="131"/>
-      <c r="G40" s="131"/>
-      <c r="H40" s="131"/>
-      <c r="I40" s="131" t="s">
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="111"/>
+      <c r="G40" s="111"/>
+      <c r="H40" s="111"/>
+      <c r="I40" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="J40" s="131"/>
-      <c r="K40" s="131"/>
-      <c r="L40" s="131"/>
-      <c r="M40" s="128"/>
-      <c r="N40" s="128"/>
-      <c r="O40" s="128"/>
-      <c r="P40" s="128"/>
-      <c r="S40" s="121" t="s">
+      <c r="J40" s="111"/>
+      <c r="K40" s="111"/>
+      <c r="L40" s="111"/>
+      <c r="M40" s="108"/>
+      <c r="N40" s="108"/>
+      <c r="O40" s="108"/>
+      <c r="P40" s="108"/>
+      <c r="S40" s="114" t="s">
         <v>79</v>
       </c>
-      <c r="T40" s="121"/>
+      <c r="T40" s="114"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -5355,30 +5663,30 @@
       <c r="B41" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="130" t="s">
+      <c r="C41" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="130"/>
-      <c r="E41" s="130"/>
-      <c r="F41" s="130" t="s">
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112" t="s">
         <v>61</v>
       </c>
-      <c r="G41" s="130"/>
-      <c r="H41" s="130"/>
-      <c r="I41" s="130" t="s">
+      <c r="G41" s="112"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="J41" s="130"/>
-      <c r="K41" s="130"/>
-      <c r="L41" s="130"/>
-      <c r="M41" s="129"/>
-      <c r="N41" s="129"/>
-      <c r="O41" s="129"/>
-      <c r="P41" s="129"/>
-      <c r="S41" s="121" t="s">
+      <c r="J41" s="112"/>
+      <c r="K41" s="112"/>
+      <c r="L41" s="112"/>
+      <c r="M41" s="109"/>
+      <c r="N41" s="109"/>
+      <c r="O41" s="109"/>
+      <c r="P41" s="109"/>
+      <c r="S41" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="T41" s="121"/>
+      <c r="T41" s="114"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
@@ -5391,30 +5699,30 @@
       <c r="B42" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="130" t="s">
+      <c r="C42" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="130"/>
-      <c r="E42" s="130"/>
-      <c r="F42" s="130" t="s">
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="G42" s="130"/>
-      <c r="H42" s="130"/>
-      <c r="I42" s="130" t="s">
+      <c r="G42" s="112"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="J42" s="130"/>
-      <c r="K42" s="130"/>
-      <c r="L42" s="130"/>
-      <c r="M42" s="129"/>
-      <c r="N42" s="129"/>
-      <c r="O42" s="129"/>
-      <c r="P42" s="129"/>
-      <c r="S42" s="121" t="s">
+      <c r="J42" s="112"/>
+      <c r="K42" s="112"/>
+      <c r="L42" s="112"/>
+      <c r="M42" s="109"/>
+      <c r="N42" s="109"/>
+      <c r="O42" s="109"/>
+      <c r="P42" s="109"/>
+      <c r="S42" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="T42" s="121"/>
+      <c r="T42" s="114"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -5423,24 +5731,24 @@
     <row r="43" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
-      <c r="C43" s="127"/>
-      <c r="D43" s="127"/>
-      <c r="E43" s="127"/>
-      <c r="F43" s="127"/>
-      <c r="G43" s="127"/>
-      <c r="H43" s="127"/>
-      <c r="I43" s="127"/>
-      <c r="J43" s="127"/>
-      <c r="K43" s="127"/>
-      <c r="L43" s="127"/>
+      <c r="C43" s="110"/>
+      <c r="D43" s="110"/>
+      <c r="E43" s="110"/>
+      <c r="F43" s="110"/>
+      <c r="G43" s="110"/>
+      <c r="H43" s="110"/>
+      <c r="I43" s="110"/>
+      <c r="J43" s="110"/>
+      <c r="K43" s="110"/>
+      <c r="L43" s="110"/>
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
-      <c r="O43" s="129"/>
-      <c r="P43" s="129"/>
-      <c r="S43" s="121" t="s">
+      <c r="O43" s="109"/>
+      <c r="P43" s="109"/>
+      <c r="S43" s="114" t="s">
         <v>100</v>
       </c>
-      <c r="T43" s="121"/>
+      <c r="T43" s="114"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -5451,211 +5759,277 @@
     <row r="44" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
-      <c r="C44" s="127"/>
-      <c r="D44" s="127"/>
-      <c r="E44" s="127"/>
-      <c r="F44" s="127"/>
-      <c r="G44" s="127"/>
-      <c r="H44" s="127"/>
-      <c r="I44" s="127"/>
-      <c r="J44" s="127"/>
-      <c r="K44" s="127"/>
-      <c r="L44" s="127"/>
+      <c r="C44" s="110"/>
+      <c r="D44" s="110"/>
+      <c r="E44" s="110"/>
+      <c r="F44" s="110"/>
+      <c r="G44" s="110"/>
+      <c r="H44" s="110"/>
+      <c r="I44" s="110"/>
+      <c r="J44" s="110"/>
+      <c r="K44" s="110"/>
+      <c r="L44" s="110"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
-      <c r="O44" s="129"/>
-      <c r="P44" s="129"/>
+      <c r="O44" s="109"/>
+      <c r="P44" s="109"/>
       <c r="S44" s="57"/>
       <c r="T44" s="57"/>
       <c r="U44" s="57"/>
     </row>
     <row r="45" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="46" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="47" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="48" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="35"/>
+      <c r="B47" s="77" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47" s="111" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47" s="111"/>
+      <c r="E47" s="111" t="s">
+        <v>196</v>
+      </c>
+      <c r="F47" s="111"/>
+      <c r="G47" s="111"/>
+      <c r="H47" s="111"/>
+      <c r="I47" s="134"/>
+      <c r="J47" s="134"/>
+    </row>
+    <row r="48" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="38" t="e" vm="25">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B48" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" s="112">
+        <v>2</v>
+      </c>
+      <c r="D48" s="112"/>
+      <c r="E48" s="112" t="s">
+        <v>201</v>
+      </c>
+      <c r="F48" s="112"/>
+      <c r="G48" s="112"/>
+      <c r="H48" s="112"/>
+      <c r="I48" s="133"/>
+      <c r="J48" s="133"/>
+    </row>
     <row r="49" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="58" t="s">
+      <c r="A49" s="38" t="e" vm="26">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B49" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" s="112" t="s">
+        <v>200</v>
+      </c>
+      <c r="D49" s="112"/>
+      <c r="E49" s="112" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" s="112"/>
+      <c r="G49" s="112"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="133"/>
+      <c r="J49" s="133"/>
+    </row>
+    <row r="50" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="110"/>
+      <c r="D50" s="110"/>
+      <c r="E50" s="110"/>
+      <c r="F50" s="110"/>
+      <c r="G50" s="110"/>
+      <c r="H50" s="110"/>
+      <c r="I50" s="132"/>
+      <c r="J50" s="132"/>
+    </row>
+    <row r="51" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="58" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="51" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C51" s="63" t="s">
+    <row r="54" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C54" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D54" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="H51" s="123" t="s">
+      <c r="H54" s="123" t="s">
         <v>70</v>
       </c>
-      <c r="I51" s="123"/>
-      <c r="J51" s="123"/>
-      <c r="K51" s="123"/>
-      <c r="L51" s="123"/>
-      <c r="M51" s="123"/>
-    </row>
-    <row r="52" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="91"/>
-      <c r="B52" s="87" t="s">
+      <c r="I54" s="123"/>
+      <c r="J54" s="123"/>
+      <c r="K54" s="123"/>
+      <c r="L54" s="123"/>
+      <c r="M54" s="123"/>
+    </row>
+    <row r="55" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="91"/>
+      <c r="B55" s="87" t="s">
         <v>175</v>
       </c>
-      <c r="C52" s="88">
+      <c r="C55" s="88">
         <v>-1</v>
       </c>
-      <c r="D52" s="88">
+      <c r="D55" s="88">
         <v>0</v>
       </c>
-      <c r="E52" s="88">
+      <c r="E55" s="88">
         <v>1</v>
       </c>
-      <c r="F52" s="88">
+      <c r="F55" s="88">
         <v>2</v>
       </c>
-      <c r="G52" s="88">
+      <c r="G55" s="88">
         <v>3</v>
       </c>
-      <c r="H52" s="89">
+      <c r="H55" s="89">
         <v>4</v>
       </c>
-      <c r="I52" s="89">
+      <c r="I55" s="89">
         <v>5</v>
       </c>
-      <c r="J52" s="89">
+      <c r="J55" s="89">
         <v>6</v>
       </c>
-      <c r="K52" s="89">
+      <c r="K55" s="89">
         <v>7</v>
       </c>
-      <c r="L52" s="89">
+      <c r="L55" s="89">
         <v>8</v>
       </c>
-      <c r="M52" s="89">
+      <c r="M55" s="89">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="90"/>
-      <c r="B53" s="90" t="s">
+    <row r="56" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="90"/>
+      <c r="B56" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="C53" s="19">
-        <f t="shared" ref="C53:L53" si="14">(2+C52)*tilesize</f>
+      <c r="C56" s="19">
+        <f>(2+C55)*tilesize</f>
         <v>128</v>
       </c>
-      <c r="D53" s="19">
-        <f t="shared" si="14"/>
+      <c r="D56" s="19">
+        <f>(2+D55)*tilesize</f>
         <v>256</v>
       </c>
-      <c r="E53" s="19">
-        <f t="shared" si="14"/>
+      <c r="E56" s="19">
+        <f>(2+E55)*tilesize</f>
         <v>384</v>
       </c>
-      <c r="F53" s="19">
-        <f t="shared" si="14"/>
+      <c r="F56" s="19">
+        <f>(2+F55)*tilesize</f>
         <v>512</v>
       </c>
-      <c r="G53" s="19">
-        <f t="shared" si="14"/>
+      <c r="G56" s="19">
+        <f>(2+G55)*tilesize</f>
         <v>640</v>
       </c>
-      <c r="H53" s="19">
-        <f t="shared" si="14"/>
+      <c r="H56" s="19">
+        <f>(2+H55)*tilesize</f>
         <v>768</v>
       </c>
-      <c r="I53" s="19">
-        <f t="shared" si="14"/>
+      <c r="I56" s="19">
+        <f>(2+I55)*tilesize</f>
         <v>896</v>
       </c>
-      <c r="J53" s="19">
-        <f t="shared" si="14"/>
+      <c r="J56" s="19">
+        <f>(2+J55)*tilesize</f>
         <v>1024</v>
       </c>
-      <c r="K53" s="19">
-        <f t="shared" si="14"/>
+      <c r="K56" s="19">
+        <f>(2+K55)*tilesize</f>
         <v>1152</v>
       </c>
-      <c r="L53" s="19">
-        <f t="shared" si="14"/>
+      <c r="L56" s="19">
+        <f>(2+L55)*tilesize</f>
         <v>1280</v>
       </c>
-      <c r="M53" s="19">
-        <f>(2+M52)*tilesize</f>
+      <c r="M56" s="19">
+        <f>(2+M55)*tilesize</f>
         <v>1408</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="90"/>
-      <c r="B54" s="90" t="s">
+    <row r="57" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="90"/>
+      <c r="B57" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="C54" s="51">
-        <f t="shared" ref="C54:M54" si="15">(2+C52+1)*tilesize+tilesize/2</f>
+      <c r="C57" s="51">
+        <f>(2+C55+1)*tilesize+tilesize/2</f>
         <v>320</v>
       </c>
-      <c r="D54" s="52">
-        <f t="shared" si="15"/>
+      <c r="D57" s="52">
+        <f>(2+D55+1)*tilesize+tilesize/2</f>
         <v>448</v>
       </c>
-      <c r="E54" s="48">
-        <f t="shared" si="15"/>
+      <c r="E57" s="48">
+        <f>(2+E55+1)*tilesize+tilesize/2</f>
         <v>576</v>
       </c>
-      <c r="F54" s="50">
-        <f t="shared" si="15"/>
+      <c r="F57" s="50">
+        <f>(2+F55+1)*tilesize+tilesize/2</f>
         <v>704</v>
       </c>
-      <c r="G54" s="49">
-        <f t="shared" si="15"/>
+      <c r="G57" s="49">
+        <f>(2+G55+1)*tilesize+tilesize/2</f>
         <v>832</v>
       </c>
-      <c r="H54" s="92">
-        <f t="shared" si="15"/>
+      <c r="H57" s="92">
+        <f>(2+H55+1)*tilesize+tilesize/2</f>
         <v>960</v>
       </c>
-      <c r="I54" s="46">
-        <f t="shared" si="15"/>
+      <c r="I57" s="46">
+        <f>(2+I55+1)*tilesize+tilesize/2</f>
         <v>1088</v>
       </c>
-      <c r="J54" s="47">
-        <f t="shared" si="15"/>
+      <c r="J57" s="47">
+        <f>(2+J55+1)*tilesize+tilesize/2</f>
         <v>1216</v>
       </c>
-      <c r="K54" s="93">
-        <f t="shared" si="15"/>
+      <c r="K57" s="93">
+        <f>(2+K55+1)*tilesize+tilesize/2</f>
         <v>1344</v>
       </c>
-      <c r="L54" s="45">
-        <f t="shared" si="15"/>
+      <c r="L57" s="45">
+        <f>(2+L55+1)*tilesize+tilesize/2</f>
         <v>1472</v>
       </c>
-      <c r="M54" s="42">
-        <f t="shared" si="15"/>
+      <c r="M57" s="42">
+        <f>(2+M55+1)*tilesize+tilesize/2</f>
         <v>1600</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C55" s="64" t="s">
+    <row r="58" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C58" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="D55" s="60" t="s">
+      <c r="D58" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="E55" s="61"/>
-      <c r="F55" s="62"/>
-      <c r="G55" s="57"/>
-      <c r="H55" s="124" t="s">
+      <c r="E58" s="61"/>
+      <c r="F58" s="62"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="124" t="s">
         <v>167</v>
       </c>
-      <c r="I55" s="124"/>
-      <c r="J55" s="124"/>
-      <c r="K55" s="124"/>
-      <c r="L55" s="124"/>
-      <c r="M55" s="124"/>
-    </row>
-    <row r="56" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="57" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="58" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
+      <c r="I58" s="124"/>
+      <c r="J58" s="124"/>
+      <c r="K58" s="124"/>
+      <c r="L58" s="124"/>
+      <c r="M58" s="124"/>
+    </row>
     <row r="59" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="60" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="O60" t="s">
@@ -5703,10 +6077,10 @@
       <c r="I62" t="s">
         <v>98</v>
       </c>
-      <c r="J62" s="112" t="s">
+      <c r="J62" s="129" t="s">
         <v>102</v>
       </c>
-      <c r="K62" s="112"/>
+      <c r="K62" s="129"/>
       <c r="L62" t="s">
         <v>103</v>
       </c>
@@ -5714,20 +6088,20 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>23</v>
       </c>
-      <c r="O62" s="111" t="s">
+      <c r="O62" s="128" t="s">
         <v>108</v>
       </c>
-      <c r="P62" s="111"/>
-      <c r="Q62" s="111"/>
-      <c r="R62" s="111"/>
-      <c r="S62" s="111"/>
+      <c r="P62" s="128"/>
+      <c r="Q62" s="128"/>
+      <c r="R62" s="128"/>
+      <c r="S62" s="128"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
       <c r="AJ62" s="81"/>
     </row>
     <row r="63" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="91" t="e" vm="25">
+      <c r="A63" s="91" t="e" vm="27">
         <v>#VALUE!</v>
       </c>
       <c r="B63" s="85" t="s">
@@ -5742,20 +6116,20 @@
       <c r="E63" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="F63" s="113" t="s">
+      <c r="F63" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="G63" s="113"/>
+      <c r="G63" s="116"/>
       <c r="H63" s="86" t="s">
         <v>193</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="113" t="s">
+      <c r="J63" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="K63" s="113"/>
+      <c r="K63" s="116"/>
       <c r="L63" s="86" t="s">
         <v>104</v>
       </c>
@@ -5779,10 +6153,10 @@
         <v>115</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="113" t="s">
+      <c r="U63" s="116" t="s">
         <v>119</v>
       </c>
-      <c r="V63" s="113"/>
+      <c r="V63" s="116"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -5821,7 +6195,7 @@
         <v>0</v>
       </c>
       <c r="J64" s="117">
-        <f t="shared" ref="J64:J69" si="16">(C64-player_radius)*2</f>
+        <f t="shared" ref="J64:J69" si="14">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
       <c r="K64" s="117"/>
@@ -5835,19 +6209,19 @@
       </c>
       <c r="N64" s="97"/>
       <c r="O64" s="99">
-        <f t="shared" ref="O64:O70" si="17">ROUND(D64/health_cap,2)*10</f>
+        <f t="shared" ref="O64:O70" si="15">ROUND(D64/health_cap,2)*10</f>
         <v>0.8</v>
       </c>
       <c r="P64" s="100">
-        <f t="shared" ref="P64:P70" si="18">ROUND(M64/guns_cap,2)*10</f>
+        <f t="shared" ref="P64:P70" si="16">ROUND(M64/guns_cap,2)*10</f>
         <v>3.3000000000000003</v>
       </c>
       <c r="Q64" s="101">
-        <f t="shared" ref="Q64:Q70" si="19">ROUND(E64/speed_cap,2)*10</f>
+        <f t="shared" ref="Q64:Q70" si="17">ROUND(E64/speed_cap,2)*10</f>
         <v>6</v>
       </c>
       <c r="R64" s="102">
-        <f t="shared" ref="R64:R70" si="20">ROUND(I64/DPS_cap,2)*10</f>
+        <f t="shared" ref="R64:R70" si="18">ROUND(I64/DPS_cap,2)*10</f>
         <v>0</v>
       </c>
       <c r="S64" s="103">
@@ -5855,11 +6229,11 @@
         <v>10.100000000000001</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="114">
+      <c r="U64" s="130">
         <f>R64+O64+P64</f>
         <v>4.1000000000000005</v>
       </c>
-      <c r="V64" s="114"/>
+      <c r="V64" s="130"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -5887,10 +6261,10 @@
       <c r="E65" s="54">
         <v>3</v>
       </c>
-      <c r="F65" s="108" t="s">
+      <c r="F65" s="120" t="s">
         <v>97</v>
       </c>
-      <c r="G65" s="108"/>
+      <c r="G65" s="120"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
@@ -5898,7 +6272,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="117">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>32</v>
       </c>
       <c r="K65" s="117"/>
@@ -5907,36 +6281,36 @@
         <v>2</v>
       </c>
       <c r="M65" s="54">
-        <f t="shared" ref="M65:M68" si="21">21-L65</f>
+        <f t="shared" ref="M65:M68" si="19">21-L65</f>
         <v>19</v>
       </c>
       <c r="N65" s="54"/>
       <c r="O65" s="66">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="P65" s="67">
+        <f t="shared" si="16"/>
+        <v>6.3</v>
+      </c>
+      <c r="Q65" s="68">
         <f t="shared" si="17"/>
         <v>3</v>
       </c>
-      <c r="P65" s="67">
+      <c r="R65" s="69">
         <f t="shared" si="18"/>
-        <v>6.3</v>
-      </c>
-      <c r="Q65" s="68">
-        <f t="shared" si="19"/>
-        <v>3</v>
-      </c>
-      <c r="R65" s="69">
-        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="S65" s="70">
-        <f t="shared" ref="S65:S69" si="22">SUM(O65:R65)</f>
+        <f t="shared" ref="S65:S69" si="20">SUM(O65:R65)</f>
         <v>12.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="115">
-        <f t="shared" ref="U65:U70" si="23">R65+O65+P65</f>
+      <c r="U65" s="127">
+        <f t="shared" ref="U65:U70" si="21">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="115"/>
+      <c r="V65" s="127"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -5964,10 +6338,10 @@
       <c r="E66" s="54">
         <v>4</v>
       </c>
-      <c r="F66" s="108" t="s">
+      <c r="F66" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="108"/>
+      <c r="G66" s="120"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
@@ -5975,7 +6349,7 @@
         <v>11.11</v>
       </c>
       <c r="J66" s="117">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>28</v>
       </c>
       <c r="K66" s="117"/>
@@ -5984,36 +6358,36 @@
         <v>4</v>
       </c>
       <c r="M66" s="54">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>17</v>
       </c>
       <c r="N66" s="54"/>
       <c r="O66" s="66">
+        <f t="shared" si="15"/>
+        <v>2.5</v>
+      </c>
+      <c r="P66" s="67">
+        <f t="shared" si="16"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="Q66" s="68">
         <f t="shared" si="17"/>
-        <v>2.5</v>
-      </c>
-      <c r="P66" s="67">
+        <v>4</v>
+      </c>
+      <c r="R66" s="69">
         <f t="shared" si="18"/>
-        <v>5.6999999999999993</v>
-      </c>
-      <c r="Q66" s="68">
-        <f t="shared" si="19"/>
-        <v>4</v>
-      </c>
-      <c r="R66" s="69">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S66" s="70">
         <f t="shared" si="20"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="S66" s="70">
-        <f t="shared" si="22"/>
         <v>14.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="115">
-        <f t="shared" si="23"/>
+      <c r="U66" s="127">
+        <f t="shared" si="21"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="115"/>
+      <c r="V66" s="127"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6041,10 +6415,10 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="108" t="s">
+      <c r="F67" s="120" t="s">
         <v>96</v>
       </c>
-      <c r="G67" s="108"/>
+      <c r="G67" s="120"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
@@ -6052,7 +6426,7 @@
         <v>5.63</v>
       </c>
       <c r="J67" s="117">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>48</v>
       </c>
       <c r="K67" s="117"/>
@@ -6061,36 +6435,36 @@
         <v>0</v>
       </c>
       <c r="M67" s="54">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>21</v>
       </c>
       <c r="N67" s="54"/>
       <c r="O67" s="66">
+        <f t="shared" si="15"/>
+        <v>9.6</v>
+      </c>
+      <c r="P67" s="67">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="Q67" s="68">
         <f t="shared" si="17"/>
-        <v>9.6</v>
-      </c>
-      <c r="P67" s="67">
+        <v>1</v>
+      </c>
+      <c r="R67" s="69">
         <f t="shared" si="18"/>
-        <v>7</v>
-      </c>
-      <c r="Q67" s="68">
-        <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-      <c r="R67" s="69">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S67" s="70">
         <f t="shared" si="20"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="S67" s="70">
-        <f t="shared" si="22"/>
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="115">
-        <f t="shared" si="23"/>
+      <c r="U67" s="127">
+        <f t="shared" si="21"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="115"/>
+      <c r="V67" s="127"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6114,10 +6488,10 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="108" t="s">
+      <c r="F68" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="108"/>
+      <c r="G68" s="120"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
@@ -6125,7 +6499,7 @@
         <v>13.33</v>
       </c>
       <c r="J68" s="117">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>72</v>
       </c>
       <c r="K68" s="117"/>
@@ -6134,36 +6508,36 @@
         <v>0</v>
       </c>
       <c r="M68" s="54">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>21</v>
       </c>
       <c r="N68" s="54"/>
       <c r="O68" s="66">
+        <f t="shared" si="15"/>
+        <v>7.4</v>
+      </c>
+      <c r="P68" s="67">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="Q68" s="68">
         <f t="shared" si="17"/>
-        <v>7.4</v>
-      </c>
-      <c r="P68" s="67">
+        <v>0</v>
+      </c>
+      <c r="R68" s="69">
         <f t="shared" si="18"/>
-        <v>7</v>
-      </c>
-      <c r="Q68" s="68">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R68" s="69">
+        <v>2.7</v>
+      </c>
+      <c r="S68" s="70">
         <f t="shared" si="20"/>
-        <v>2.7</v>
-      </c>
-      <c r="S68" s="70">
-        <f t="shared" si="22"/>
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="115">
-        <f t="shared" si="23"/>
+      <c r="U68" s="127">
+        <f t="shared" si="21"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="115"/>
+      <c r="V68" s="127"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -6187,10 +6561,10 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="108" t="s">
+      <c r="F69" s="120" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="108"/>
+      <c r="G69" s="120"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
@@ -6198,7 +6572,7 @@
         <v>9.09</v>
       </c>
       <c r="J69" s="117">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>20</v>
       </c>
       <c r="K69" s="117"/>
@@ -6212,31 +6586,31 @@
       </c>
       <c r="N69" s="54"/>
       <c r="O69" s="66">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="P69" s="67">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="Q69" s="68">
         <f t="shared" si="17"/>
-        <v>2</v>
-      </c>
-      <c r="P69" s="67">
+        <v>10</v>
+      </c>
+      <c r="R69" s="69">
         <f t="shared" si="18"/>
-        <v>5</v>
-      </c>
-      <c r="Q69" s="68">
-        <f t="shared" si="19"/>
-        <v>10</v>
-      </c>
-      <c r="R69" s="69">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="S69" s="70">
         <f t="shared" si="20"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="S69" s="70">
-        <f t="shared" si="22"/>
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="115">
-        <f t="shared" si="23"/>
+      <c r="U69" s="127">
+        <f t="shared" si="21"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="115"/>
+      <c r="V69" s="127"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -6260,10 +6634,10 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="108" t="s">
+      <c r="F70" s="120" t="s">
         <v>118</v>
       </c>
-      <c r="G70" s="108"/>
+      <c r="G70" s="120"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
@@ -6271,7 +6645,7 @@
         <v>48</v>
       </c>
       <c r="J70" s="117">
-        <f t="shared" ref="J70" si="24">(C70-player_radius)*2</f>
+        <f t="shared" ref="J70" si="22">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
       <c r="K70" s="117"/>
@@ -6285,31 +6659,31 @@
       </c>
       <c r="N70" s="54"/>
       <c r="O70" s="66">
+        <f t="shared" si="15"/>
+        <v>2.5</v>
+      </c>
+      <c r="P70" s="67">
+        <f t="shared" si="16"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="Q70" s="68">
         <f t="shared" si="17"/>
-        <v>2.5</v>
-      </c>
-      <c r="P70" s="67">
+        <v>8</v>
+      </c>
+      <c r="R70" s="69">
         <f t="shared" si="18"/>
-        <v>5.6999999999999993</v>
-      </c>
-      <c r="Q70" s="68">
-        <f t="shared" si="19"/>
-        <v>8</v>
-      </c>
-      <c r="R70" s="69">
-        <f t="shared" si="20"/>
         <v>9.6</v>
       </c>
       <c r="S70" s="70">
-        <f t="shared" ref="S70" si="25">SUM(O70:R70)</f>
+        <f t="shared" ref="S70" si="23">SUM(O70:R70)</f>
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="115">
-        <f t="shared" si="23"/>
+      <c r="U70" s="127">
+        <f t="shared" si="21"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="115"/>
+      <c r="V70" s="127"/>
       <c r="W70" s="25" t="s">
         <v>76</v>
       </c>
@@ -6322,12 +6696,12 @@
     <row r="71" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="72" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="73" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="O73" s="118" t="s">
+      <c r="O73" s="121" t="s">
         <v>170</v>
       </c>
-      <c r="P73" s="118"/>
-      <c r="Q73" s="118"/>
-      <c r="R73" s="118"/>
+      <c r="P73" s="121"/>
+      <c r="Q73" s="121"/>
+      <c r="R73" s="121"/>
     </row>
     <row r="74" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="35"/>
@@ -6343,34 +6717,34 @@
       <c r="E74" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="F74" s="110" t="s">
+      <c r="F74" s="119" t="s">
         <v>138</v>
       </c>
-      <c r="G74" s="110"/>
-      <c r="H74" s="110" t="s">
+      <c r="G74" s="119"/>
+      <c r="H74" s="119" t="s">
         <v>139</v>
       </c>
-      <c r="I74" s="110"/>
-      <c r="J74" s="110" t="s">
+      <c r="I74" s="119"/>
+      <c r="J74" s="119" t="s">
         <v>136</v>
       </c>
-      <c r="K74" s="110"/>
-      <c r="L74" s="110"/>
-      <c r="M74" s="110"/>
+      <c r="K74" s="119"/>
+      <c r="L74" s="119"/>
+      <c r="M74" s="119"/>
       <c r="N74" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="O74" s="110" t="s">
+      <c r="O74" s="119" t="s">
         <v>172</v>
       </c>
-      <c r="P74" s="110"/>
-      <c r="Q74" s="110" t="s">
+      <c r="P74" s="119"/>
+      <c r="Q74" s="119" t="s">
         <v>173</v>
       </c>
-      <c r="R74" s="110"/>
+      <c r="R74" s="119"/>
     </row>
     <row r="75" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="38" t="e" vm="26">
+      <c r="A75" s="38" t="e" vm="28">
         <v>#VALUE!</v>
       </c>
       <c r="B75" s="38" t="s">
@@ -6400,20 +6774,20 @@
       <c r="K75" s="117"/>
       <c r="L75" s="117"/>
       <c r="M75" s="117"/>
-      <c r="N75" s="78" t="e" vm="27">
+      <c r="N75" s="78" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
-      <c r="O75" s="70" t="e" vm="28">
+      <c r="O75" s="70" t="e" vm="30">
         <v>#VALUE!</v>
       </c>
-      <c r="P75" s="70" t="e" vm="29">
+      <c r="P75" s="70" t="e" vm="31">
         <v>#VALUE!</v>
       </c>
       <c r="Q75" s="79"/>
       <c r="R75" s="95"/>
     </row>
     <row r="76" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="38" t="e" vm="30">
+      <c r="A76" s="38" t="e" vm="32">
         <v>#VALUE!</v>
       </c>
       <c r="B76" s="38" t="s">
@@ -6443,13 +6817,13 @@
       <c r="K76" s="117"/>
       <c r="L76" s="117"/>
       <c r="M76" s="117"/>
-      <c r="N76" s="78" t="e" vm="31">
+      <c r="N76" s="78" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
-      <c r="O76" s="70" t="e" vm="32">
+      <c r="O76" s="70" t="e" vm="34">
         <v>#VALUE!</v>
       </c>
-      <c r="P76" s="70" t="e" vm="33">
+      <c r="P76" s="70" t="e" vm="35">
         <v>#VALUE!</v>
       </c>
       <c r="Q76" s="79"/>
@@ -6461,24 +6835,24 @@
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
       <c r="E77" s="44"/>
-      <c r="F77" s="127"/>
-      <c r="G77" s="127"/>
-      <c r="H77" s="127"/>
-      <c r="I77" s="127"/>
-      <c r="J77" s="127"/>
-      <c r="K77" s="127"/>
-      <c r="L77" s="127"/>
-      <c r="M77" s="127"/>
+      <c r="F77" s="110"/>
+      <c r="G77" s="110"/>
+      <c r="H77" s="110"/>
+      <c r="I77" s="110"/>
+      <c r="J77" s="110"/>
+      <c r="K77" s="110"/>
+      <c r="L77" s="110"/>
+      <c r="M77" s="110"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="125"/>
-      <c r="P77" s="125"/>
-      <c r="Q77" s="125"/>
-      <c r="R77" s="125"/>
+      <c r="O77" s="118"/>
+      <c r="P77" s="118"/>
+      <c r="Q77" s="118"/>
+      <c r="R77" s="118"/>
     </row>
     <row r="78" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="79" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="80" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="35" t="e" vm="34">
+      <c r="A80" s="35" t="e" vm="36">
         <v>#VALUE!</v>
       </c>
       <c r="B80" s="77" t="s">
@@ -6493,32 +6867,32 @@
       <c r="E80" s="107" t="s">
         <v>147</v>
       </c>
-      <c r="F80" s="110" t="s">
+      <c r="F80" s="119" t="s">
         <v>142</v>
       </c>
-      <c r="G80" s="110"/>
-      <c r="H80" s="110"/>
-      <c r="I80" s="110"/>
-      <c r="J80" s="110"/>
-      <c r="K80" s="110"/>
-      <c r="L80" s="110"/>
-      <c r="M80" s="110"/>
-      <c r="N80" s="110"/>
-      <c r="O80" s="110"/>
-      <c r="P80" s="110"/>
-      <c r="Q80" s="110" t="s">
+      <c r="G80" s="119"/>
+      <c r="H80" s="119"/>
+      <c r="I80" s="119"/>
+      <c r="J80" s="119"/>
+      <c r="K80" s="119"/>
+      <c r="L80" s="119"/>
+      <c r="M80" s="119"/>
+      <c r="N80" s="119"/>
+      <c r="O80" s="119"/>
+      <c r="P80" s="119"/>
+      <c r="Q80" s="119" t="s">
         <v>157</v>
       </c>
-      <c r="R80" s="110"/>
-      <c r="S80" s="110"/>
-      <c r="T80" s="110"/>
-      <c r="U80" s="110"/>
-      <c r="V80" s="110"/>
-      <c r="W80" s="110"/>
-      <c r="X80" s="110"/>
-      <c r="Y80" s="110"/>
-      <c r="Z80" s="110"/>
-      <c r="AA80" s="110"/>
+      <c r="R80" s="119"/>
+      <c r="S80" s="119"/>
+      <c r="T80" s="119"/>
+      <c r="U80" s="119"/>
+      <c r="V80" s="119"/>
+      <c r="W80" s="119"/>
+      <c r="X80" s="119"/>
+      <c r="Y80" s="119"/>
+      <c r="Z80" s="119"/>
+      <c r="AA80" s="119"/>
     </row>
     <row r="81" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="38"/>
@@ -6534,32 +6908,32 @@
       <c r="E81" s="97">
         <v>16</v>
       </c>
-      <c r="F81" s="116" t="s">
+      <c r="F81" s="126" t="s">
         <v>153</v>
       </c>
-      <c r="G81" s="116"/>
-      <c r="H81" s="116"/>
-      <c r="I81" s="116"/>
-      <c r="J81" s="116"/>
-      <c r="K81" s="116"/>
-      <c r="L81" s="116"/>
-      <c r="M81" s="116"/>
-      <c r="N81" s="116"/>
-      <c r="O81" s="116"/>
-      <c r="P81" s="116"/>
-      <c r="Q81" s="116" t="s">
+      <c r="G81" s="126"/>
+      <c r="H81" s="126"/>
+      <c r="I81" s="126"/>
+      <c r="J81" s="126"/>
+      <c r="K81" s="126"/>
+      <c r="L81" s="126"/>
+      <c r="M81" s="126"/>
+      <c r="N81" s="126"/>
+      <c r="O81" s="126"/>
+      <c r="P81" s="126"/>
+      <c r="Q81" s="126" t="s">
         <v>158</v>
       </c>
-      <c r="R81" s="116"/>
-      <c r="S81" s="116"/>
-      <c r="T81" s="116"/>
-      <c r="U81" s="116"/>
-      <c r="V81" s="116"/>
-      <c r="W81" s="116"/>
-      <c r="X81" s="116"/>
-      <c r="Y81" s="116"/>
-      <c r="Z81" s="116"/>
-      <c r="AA81" s="116"/>
+      <c r="R81" s="126"/>
+      <c r="S81" s="126"/>
+      <c r="T81" s="126"/>
+      <c r="U81" s="126"/>
+      <c r="V81" s="126"/>
+      <c r="W81" s="126"/>
+      <c r="X81" s="126"/>
+      <c r="Y81" s="126"/>
+      <c r="Z81" s="126"/>
+      <c r="AA81" s="126"/>
     </row>
     <row r="82" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="38"/>
@@ -6575,30 +6949,30 @@
       <c r="E82" s="54">
         <v>1</v>
       </c>
-      <c r="F82" s="119" t="s">
+      <c r="F82" s="125" t="s">
         <v>155</v>
       </c>
-      <c r="G82" s="119"/>
-      <c r="H82" s="119"/>
-      <c r="I82" s="119"/>
-      <c r="J82" s="119"/>
-      <c r="K82" s="119"/>
-      <c r="L82" s="119"/>
-      <c r="M82" s="119"/>
-      <c r="N82" s="119"/>
-      <c r="O82" s="119"/>
-      <c r="P82" s="119"/>
-      <c r="Q82" s="119"/>
-      <c r="R82" s="119"/>
-      <c r="S82" s="119"/>
-      <c r="T82" s="119"/>
-      <c r="U82" s="119"/>
-      <c r="V82" s="119"/>
-      <c r="W82" s="119"/>
-      <c r="X82" s="119"/>
-      <c r="Y82" s="119"/>
-      <c r="Z82" s="119"/>
-      <c r="AA82" s="119"/>
+      <c r="G82" s="125"/>
+      <c r="H82" s="125"/>
+      <c r="I82" s="125"/>
+      <c r="J82" s="125"/>
+      <c r="K82" s="125"/>
+      <c r="L82" s="125"/>
+      <c r="M82" s="125"/>
+      <c r="N82" s="125"/>
+      <c r="O82" s="125"/>
+      <c r="P82" s="125"/>
+      <c r="Q82" s="125"/>
+      <c r="R82" s="125"/>
+      <c r="S82" s="125"/>
+      <c r="T82" s="125"/>
+      <c r="U82" s="125"/>
+      <c r="V82" s="125"/>
+      <c r="W82" s="125"/>
+      <c r="X82" s="125"/>
+      <c r="Y82" s="125"/>
+      <c r="Z82" s="125"/>
+      <c r="AA82" s="125"/>
     </row>
     <row r="83" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="38"/>
@@ -6614,30 +6988,30 @@
       <c r="E83" s="54">
         <v>1</v>
       </c>
-      <c r="F83" s="119" t="s">
+      <c r="F83" s="125" t="s">
         <v>154</v>
       </c>
-      <c r="G83" s="119"/>
-      <c r="H83" s="119"/>
-      <c r="I83" s="119"/>
-      <c r="J83" s="119"/>
-      <c r="K83" s="119"/>
-      <c r="L83" s="119"/>
-      <c r="M83" s="119"/>
-      <c r="N83" s="119"/>
-      <c r="O83" s="119"/>
-      <c r="P83" s="119"/>
-      <c r="Q83" s="119"/>
-      <c r="R83" s="119"/>
-      <c r="S83" s="119"/>
-      <c r="T83" s="119"/>
-      <c r="U83" s="119"/>
-      <c r="V83" s="119"/>
-      <c r="W83" s="119"/>
-      <c r="X83" s="119"/>
-      <c r="Y83" s="119"/>
-      <c r="Z83" s="119"/>
-      <c r="AA83" s="119"/>
+      <c r="G83" s="125"/>
+      <c r="H83" s="125"/>
+      <c r="I83" s="125"/>
+      <c r="J83" s="125"/>
+      <c r="K83" s="125"/>
+      <c r="L83" s="125"/>
+      <c r="M83" s="125"/>
+      <c r="N83" s="125"/>
+      <c r="O83" s="125"/>
+      <c r="P83" s="125"/>
+      <c r="Q83" s="125"/>
+      <c r="R83" s="125"/>
+      <c r="S83" s="125"/>
+      <c r="T83" s="125"/>
+      <c r="U83" s="125"/>
+      <c r="V83" s="125"/>
+      <c r="W83" s="125"/>
+      <c r="X83" s="125"/>
+      <c r="Y83" s="125"/>
+      <c r="Z83" s="125"/>
+      <c r="AA83" s="125"/>
     </row>
     <row r="84" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="38"/>
@@ -6653,32 +7027,32 @@
       <c r="E84" s="54">
         <v>1</v>
       </c>
-      <c r="F84" s="119" t="s">
+      <c r="F84" s="125" t="s">
         <v>156</v>
       </c>
-      <c r="G84" s="119"/>
-      <c r="H84" s="119"/>
-      <c r="I84" s="119"/>
-      <c r="J84" s="119"/>
-      <c r="K84" s="119"/>
-      <c r="L84" s="119"/>
-      <c r="M84" s="119"/>
-      <c r="N84" s="119"/>
-      <c r="O84" s="119"/>
-      <c r="P84" s="119"/>
-      <c r="Q84" s="119" t="s">
+      <c r="G84" s="125"/>
+      <c r="H84" s="125"/>
+      <c r="I84" s="125"/>
+      <c r="J84" s="125"/>
+      <c r="K84" s="125"/>
+      <c r="L84" s="125"/>
+      <c r="M84" s="125"/>
+      <c r="N84" s="125"/>
+      <c r="O84" s="125"/>
+      <c r="P84" s="125"/>
+      <c r="Q84" s="125" t="s">
         <v>159</v>
       </c>
-      <c r="R84" s="119"/>
-      <c r="S84" s="119"/>
-      <c r="T84" s="119"/>
-      <c r="U84" s="119"/>
-      <c r="V84" s="119"/>
-      <c r="W84" s="119"/>
-      <c r="X84" s="119"/>
-      <c r="Y84" s="119"/>
-      <c r="Z84" s="119"/>
-      <c r="AA84" s="119"/>
+      <c r="R84" s="125"/>
+      <c r="S84" s="125"/>
+      <c r="T84" s="125"/>
+      <c r="U84" s="125"/>
+      <c r="V84" s="125"/>
+      <c r="W84" s="125"/>
+      <c r="X84" s="125"/>
+      <c r="Y84" s="125"/>
+      <c r="Z84" s="125"/>
+      <c r="AA84" s="125"/>
     </row>
     <row r="85" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="38"/>
@@ -6686,28 +7060,28 @@
       <c r="C85" s="65"/>
       <c r="D85" s="54"/>
       <c r="E85" s="54"/>
-      <c r="F85" s="119"/>
-      <c r="G85" s="119"/>
-      <c r="H85" s="119"/>
-      <c r="I85" s="119"/>
-      <c r="J85" s="119"/>
-      <c r="K85" s="119"/>
-      <c r="L85" s="119"/>
-      <c r="M85" s="119"/>
-      <c r="N85" s="119"/>
-      <c r="O85" s="119"/>
-      <c r="P85" s="119"/>
-      <c r="Q85" s="119"/>
-      <c r="R85" s="119"/>
-      <c r="S85" s="119"/>
-      <c r="T85" s="119"/>
-      <c r="U85" s="119"/>
-      <c r="V85" s="119"/>
-      <c r="W85" s="119"/>
-      <c r="X85" s="119"/>
-      <c r="Y85" s="119"/>
-      <c r="Z85" s="119"/>
-      <c r="AA85" s="119"/>
+      <c r="F85" s="125"/>
+      <c r="G85" s="125"/>
+      <c r="H85" s="125"/>
+      <c r="I85" s="125"/>
+      <c r="J85" s="125"/>
+      <c r="K85" s="125"/>
+      <c r="L85" s="125"/>
+      <c r="M85" s="125"/>
+      <c r="N85" s="125"/>
+      <c r="O85" s="125"/>
+      <c r="P85" s="125"/>
+      <c r="Q85" s="125"/>
+      <c r="R85" s="125"/>
+      <c r="S85" s="125"/>
+      <c r="T85" s="125"/>
+      <c r="U85" s="125"/>
+      <c r="V85" s="125"/>
+      <c r="W85" s="125"/>
+      <c r="X85" s="125"/>
+      <c r="Y85" s="125"/>
+      <c r="Z85" s="125"/>
+      <c r="AA85" s="125"/>
     </row>
     <row r="86" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="38"/>
@@ -6715,28 +7089,28 @@
       <c r="C86" s="65"/>
       <c r="D86" s="54"/>
       <c r="E86" s="54"/>
-      <c r="F86" s="119"/>
-      <c r="G86" s="119"/>
-      <c r="H86" s="119"/>
-      <c r="I86" s="119"/>
-      <c r="J86" s="119"/>
-      <c r="K86" s="119"/>
-      <c r="L86" s="119"/>
-      <c r="M86" s="119"/>
-      <c r="N86" s="119"/>
-      <c r="O86" s="119"/>
-      <c r="P86" s="119"/>
-      <c r="Q86" s="119"/>
-      <c r="R86" s="119"/>
-      <c r="S86" s="119"/>
-      <c r="T86" s="119"/>
-      <c r="U86" s="119"/>
-      <c r="V86" s="119"/>
-      <c r="W86" s="119"/>
-      <c r="X86" s="119"/>
-      <c r="Y86" s="119"/>
-      <c r="Z86" s="119"/>
-      <c r="AA86" s="119"/>
+      <c r="F86" s="125"/>
+      <c r="G86" s="125"/>
+      <c r="H86" s="125"/>
+      <c r="I86" s="125"/>
+      <c r="J86" s="125"/>
+      <c r="K86" s="125"/>
+      <c r="L86" s="125"/>
+      <c r="M86" s="125"/>
+      <c r="N86" s="125"/>
+      <c r="O86" s="125"/>
+      <c r="P86" s="125"/>
+      <c r="Q86" s="125"/>
+      <c r="R86" s="125"/>
+      <c r="S86" s="125"/>
+      <c r="T86" s="125"/>
+      <c r="U86" s="125"/>
+      <c r="V86" s="125"/>
+      <c r="W86" s="125"/>
+      <c r="X86" s="125"/>
+      <c r="Y86" s="125"/>
+      <c r="Z86" s="125"/>
+      <c r="AA86" s="125"/>
     </row>
     <row r="87" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="88" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6745,177 +7119,245 @@
       <c r="B89" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="C89" s="126" t="s">
+      <c r="C89" s="115" t="s">
         <v>182</v>
       </c>
-      <c r="D89" s="126"/>
-      <c r="E89" s="126"/>
-      <c r="F89" s="126"/>
-      <c r="G89" s="126"/>
-      <c r="H89" s="126" t="s">
+      <c r="D89" s="115"/>
+      <c r="E89" s="115"/>
+      <c r="F89" s="115"/>
+      <c r="G89" s="115"/>
+      <c r="H89" s="115" t="s">
         <v>142</v>
       </c>
-      <c r="I89" s="126"/>
-      <c r="J89" s="126"/>
-      <c r="K89" s="126"/>
-      <c r="L89" s="126"/>
-      <c r="M89" s="110" t="s">
+      <c r="I89" s="115"/>
+      <c r="J89" s="115"/>
+      <c r="K89" s="115"/>
+      <c r="L89" s="115"/>
+      <c r="M89" s="119" t="s">
         <v>191</v>
       </c>
-      <c r="N89" s="110"/>
+      <c r="N89" s="119"/>
       <c r="O89" s="107"/>
     </row>
     <row r="90" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="38" t="e" vm="35">
+      <c r="A90" s="38" t="e" vm="37">
         <v>#VALUE!</v>
       </c>
       <c r="B90" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C90" s="120" t="s">
+      <c r="C90" s="113" t="s">
         <v>185</v>
       </c>
-      <c r="D90" s="120"/>
-      <c r="E90" s="120"/>
-      <c r="F90" s="120"/>
-      <c r="G90" s="120"/>
-      <c r="H90" s="120" t="s">
+      <c r="D90" s="113"/>
+      <c r="E90" s="113"/>
+      <c r="F90" s="113"/>
+      <c r="G90" s="113"/>
+      <c r="H90" s="113" t="s">
         <v>187</v>
       </c>
-      <c r="I90" s="120"/>
-      <c r="J90" s="120"/>
-      <c r="K90" s="120"/>
-      <c r="L90" s="120"/>
-      <c r="M90" s="108" t="s">
+      <c r="I90" s="113"/>
+      <c r="J90" s="113"/>
+      <c r="K90" s="113"/>
+      <c r="L90" s="113"/>
+      <c r="M90" s="120" t="s">
         <v>192</v>
       </c>
-      <c r="N90" s="108"/>
+      <c r="N90" s="120"/>
       <c r="O90" s="65"/>
     </row>
     <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A91" s="38" t="e" vm="36">
+      <c r="A91" s="38" t="e" vm="38">
         <v>#VALUE!</v>
       </c>
       <c r="B91" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="C91" s="120" t="s">
+      <c r="C91" s="113" t="s">
         <v>188</v>
       </c>
-      <c r="D91" s="120"/>
-      <c r="E91" s="120"/>
-      <c r="F91" s="120"/>
-      <c r="G91" s="120"/>
-      <c r="H91" s="120" t="s">
+      <c r="D91" s="113"/>
+      <c r="E91" s="113"/>
+      <c r="F91" s="113"/>
+      <c r="G91" s="113"/>
+      <c r="H91" s="113" t="s">
         <v>190</v>
       </c>
-      <c r="I91" s="120"/>
-      <c r="J91" s="120"/>
-      <c r="K91" s="120"/>
-      <c r="L91" s="120"/>
-      <c r="M91" s="108" t="s">
+      <c r="I91" s="113"/>
+      <c r="J91" s="113"/>
+      <c r="K91" s="113"/>
+      <c r="L91" s="113"/>
+      <c r="M91" s="120" t="s">
         <v>192</v>
       </c>
-      <c r="N91" s="108"/>
+      <c r="N91" s="120"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="38" t="e" vm="37">
+      <c r="A92" s="38" t="e" vm="39">
         <v>#VALUE!</v>
       </c>
       <c r="B92" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="C92" s="120" t="s">
+      <c r="C92" s="113" t="s">
         <v>189</v>
       </c>
-      <c r="D92" s="120"/>
-      <c r="E92" s="120"/>
-      <c r="F92" s="120"/>
-      <c r="G92" s="120"/>
-      <c r="H92" s="120" t="s">
+      <c r="D92" s="113"/>
+      <c r="E92" s="113"/>
+      <c r="F92" s="113"/>
+      <c r="G92" s="113"/>
+      <c r="H92" s="113" t="s">
         <v>186</v>
       </c>
-      <c r="I92" s="120"/>
-      <c r="J92" s="120"/>
-      <c r="K92" s="120"/>
-      <c r="L92" s="120"/>
-      <c r="M92" s="108" t="s">
+      <c r="I92" s="113"/>
+      <c r="J92" s="113"/>
+      <c r="K92" s="113"/>
+      <c r="L92" s="113"/>
+      <c r="M92" s="120" t="s">
         <v>192</v>
       </c>
-      <c r="N92" s="108"/>
+      <c r="N92" s="120"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="38"/>
       <c r="B93" s="38"/>
-      <c r="C93" s="120"/>
-      <c r="D93" s="120"/>
-      <c r="E93" s="120"/>
-      <c r="F93" s="120"/>
-      <c r="G93" s="120"/>
-      <c r="H93" s="120"/>
-      <c r="I93" s="120"/>
-      <c r="J93" s="120"/>
-      <c r="K93" s="120"/>
-      <c r="L93" s="120"/>
-      <c r="M93" s="108"/>
-      <c r="N93" s="108"/>
+      <c r="C93" s="113"/>
+      <c r="D93" s="113"/>
+      <c r="E93" s="113"/>
+      <c r="F93" s="113"/>
+      <c r="G93" s="113"/>
+      <c r="H93" s="113"/>
+      <c r="I93" s="113"/>
+      <c r="J93" s="113"/>
+      <c r="K93" s="113"/>
+      <c r="L93" s="113"/>
+      <c r="M93" s="120"/>
+      <c r="N93" s="120"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="38"/>
       <c r="B94" s="38"/>
-      <c r="C94" s="120"/>
-      <c r="D94" s="120"/>
-      <c r="E94" s="120"/>
-      <c r="F94" s="120"/>
-      <c r="G94" s="120"/>
-      <c r="H94" s="120"/>
-      <c r="I94" s="120"/>
-      <c r="J94" s="120"/>
-      <c r="K94" s="120"/>
-      <c r="L94" s="120"/>
-      <c r="M94" s="108"/>
-      <c r="N94" s="108"/>
+      <c r="C94" s="113"/>
+      <c r="D94" s="113"/>
+      <c r="E94" s="113"/>
+      <c r="F94" s="113"/>
+      <c r="G94" s="113"/>
+      <c r="H94" s="113"/>
+      <c r="I94" s="113"/>
+      <c r="J94" s="113"/>
+      <c r="K94" s="113"/>
+      <c r="L94" s="113"/>
+      <c r="M94" s="120"/>
+      <c r="N94" s="120"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="38"/>
       <c r="B95" s="38"/>
-      <c r="C95" s="120"/>
-      <c r="D95" s="120"/>
-      <c r="E95" s="120"/>
-      <c r="F95" s="120"/>
-      <c r="G95" s="120"/>
-      <c r="H95" s="120"/>
-      <c r="I95" s="120"/>
-      <c r="J95" s="120"/>
-      <c r="K95" s="120"/>
-      <c r="L95" s="120"/>
-      <c r="M95" s="108"/>
-      <c r="N95" s="108"/>
+      <c r="C95" s="113"/>
+      <c r="D95" s="113"/>
+      <c r="E95" s="113"/>
+      <c r="F95" s="113"/>
+      <c r="G95" s="113"/>
+      <c r="H95" s="113"/>
+      <c r="I95" s="113"/>
+      <c r="J95" s="113"/>
+      <c r="K95" s="113"/>
+      <c r="L95" s="113"/>
+      <c r="M95" s="120"/>
+      <c r="N95" s="120"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="97" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="97" spans="2:2" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="98" spans="2:2" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B98" s="58" t="s">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="100">
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
+  <mergeCells count="108">
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M89:N89"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U64:V64"/>
+    <mergeCell ref="U65:V65"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="F80:P80"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J75:M75"/>
+    <mergeCell ref="O73:R73"/>
+    <mergeCell ref="J76:M76"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H54:M54"/>
+    <mergeCell ref="H58:M58"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q80:AA80"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="M94:N94"/>
     <mergeCell ref="C95:G95"/>
     <mergeCell ref="S42:T42"/>
     <mergeCell ref="S41:T41"/>
@@ -6932,76 +7374,20 @@
     <mergeCell ref="J77:M77"/>
     <mergeCell ref="J63:K63"/>
     <mergeCell ref="J64:K64"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H51:M51"/>
-    <mergeCell ref="H55:M55"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q80:AA80"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="U69:V69"/>
-    <mergeCell ref="U70:V70"/>
-    <mergeCell ref="F80:P80"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U68:V68"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J75:M75"/>
-    <mergeCell ref="O73:R73"/>
-    <mergeCell ref="J76:M76"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U64:V64"/>
-    <mergeCell ref="U65:V65"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M89:N89"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="F82:P82"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AWM and mk14 is darker than M1 and SLR to give difference
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1AF504-8F85-4404-950D-AA38BD64AD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C919816-3D9E-4415-8C7E-FEE49953FA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2160,74 +2160,74 @@
     <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3302,8 +3302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P78" sqref="P78"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69:K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3320,10 +3320,10 @@
       <c r="B1" s="83" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="132" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="116"/>
+      <c r="D1" s="132"/>
       <c r="G1" s="56" t="s">
         <v>163</v>
       </c>
@@ -3419,10 +3419,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="127" t="s">
+      <c r="Z2" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="127"/>
+      <c r="AA2" s="120"/>
       <c r="AG2" s="43" t="s">
         <v>86</v>
       </c>
@@ -5642,28 +5642,28 @@
       <c r="B40" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="C40" s="112" t="s">
+      <c r="C40" s="127" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="112"/>
-      <c r="E40" s="112"/>
-      <c r="F40" s="112"/>
-      <c r="G40" s="112"/>
-      <c r="H40" s="112"/>
-      <c r="I40" s="112" t="s">
+      <c r="D40" s="127"/>
+      <c r="E40" s="127"/>
+      <c r="F40" s="127"/>
+      <c r="G40" s="127"/>
+      <c r="H40" s="127"/>
+      <c r="I40" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="J40" s="112"/>
-      <c r="K40" s="112"/>
-      <c r="L40" s="112"/>
+      <c r="J40" s="127"/>
+      <c r="K40" s="127"/>
+      <c r="L40" s="127"/>
       <c r="M40" s="108"/>
       <c r="N40" s="108"/>
       <c r="O40" s="108"/>
       <c r="P40" s="108"/>
-      <c r="S40" s="128" t="s">
+      <c r="S40" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="T40" s="128"/>
+      <c r="T40" s="121"/>
       <c r="U40" s="57"/>
     </row>
     <row r="41" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -5693,10 +5693,10 @@
       <c r="N41" s="109"/>
       <c r="O41" s="109"/>
       <c r="P41" s="109"/>
-      <c r="S41" s="128" t="s">
+      <c r="S41" s="121" t="s">
         <v>77</v>
       </c>
-      <c r="T41" s="128"/>
+      <c r="T41" s="121"/>
       <c r="U41" s="57">
         <v>8</v>
       </c>
@@ -5729,10 +5729,10 @@
       <c r="N42" s="109"/>
       <c r="O42" s="109"/>
       <c r="P42" s="109"/>
-      <c r="S42" s="128" t="s">
+      <c r="S42" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="T42" s="128"/>
+      <c r="T42" s="121"/>
       <c r="U42" s="57">
         <v>128</v>
       </c>
@@ -5755,10 +5755,10 @@
       <c r="N43" s="44"/>
       <c r="O43" s="109"/>
       <c r="P43" s="109"/>
-      <c r="S43" s="128" t="s">
+      <c r="S43" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="T43" s="128"/>
+      <c r="T43" s="121"/>
       <c r="U43" s="57">
         <v>16</v>
       </c>
@@ -5794,16 +5794,16 @@
       <c r="B47" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="C47" s="112" t="s">
+      <c r="C47" s="127" t="s">
         <v>197</v>
       </c>
-      <c r="D47" s="112"/>
-      <c r="E47" s="112" t="s">
+      <c r="D47" s="127"/>
+      <c r="E47" s="127" t="s">
         <v>196</v>
       </c>
-      <c r="F47" s="112"/>
-      <c r="G47" s="112"/>
-      <c r="H47" s="112"/>
+      <c r="F47" s="127"/>
+      <c r="G47" s="127"/>
+      <c r="H47" s="127"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
     </row>
@@ -5873,14 +5873,14 @@
       <c r="D54" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="H54" s="130" t="s">
+      <c r="H54" s="124" t="s">
         <v>70</v>
       </c>
-      <c r="I54" s="130"/>
-      <c r="J54" s="130"/>
-      <c r="K54" s="130"/>
-      <c r="L54" s="130"/>
-      <c r="M54" s="130"/>
+      <c r="I54" s="124"/>
+      <c r="J54" s="124"/>
+      <c r="K54" s="124"/>
+      <c r="L54" s="124"/>
+      <c r="M54" s="124"/>
     </row>
     <row r="55" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="91"/>
@@ -6031,14 +6031,14 @@
       <c r="E58" s="61"/>
       <c r="F58" s="62"/>
       <c r="G58" s="57"/>
-      <c r="H58" s="131" t="s">
+      <c r="H58" s="125" t="s">
         <v>167</v>
       </c>
-      <c r="I58" s="131"/>
-      <c r="J58" s="131"/>
-      <c r="K58" s="131"/>
-      <c r="L58" s="131"/>
-      <c r="M58" s="131"/>
+      <c r="I58" s="125"/>
+      <c r="J58" s="125"/>
+      <c r="K58" s="125"/>
+      <c r="L58" s="125"/>
+      <c r="M58" s="125"/>
     </row>
     <row r="59" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="60" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -6087,10 +6087,10 @@
       <c r="I62" t="s">
         <v>98</v>
       </c>
-      <c r="J62" s="121" t="s">
+      <c r="J62" s="134" t="s">
         <v>102</v>
       </c>
-      <c r="K62" s="121"/>
+      <c r="K62" s="134"/>
       <c r="L62" t="s">
         <v>103</v>
       </c>
@@ -6098,13 +6098,13 @@
         <f>COUNTIF(H3:H35,"&gt;0")</f>
         <v>23</v>
       </c>
-      <c r="O62" s="120" t="s">
+      <c r="O62" s="133" t="s">
         <v>108</v>
       </c>
-      <c r="P62" s="120"/>
-      <c r="Q62" s="120"/>
-      <c r="R62" s="120"/>
-      <c r="S62" s="120"/>
+      <c r="P62" s="133"/>
+      <c r="Q62" s="133"/>
+      <c r="R62" s="133"/>
+      <c r="S62" s="133"/>
       <c r="AG62" s="81"/>
       <c r="AH62" s="81"/>
       <c r="AI62" s="81"/>
@@ -6194,10 +6194,10 @@
       <c r="E64" s="97">
         <v>6</v>
       </c>
-      <c r="F64" s="129" t="s">
+      <c r="F64" s="123" t="s">
         <v>97</v>
       </c>
-      <c r="G64" s="129"/>
+      <c r="G64" s="123"/>
       <c r="H64" s="97">
         <v>1</v>
       </c>
@@ -6239,11 +6239,11 @@
         <v>10.100000000000001</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="123">
+      <c r="U64" s="128">
         <f>R64+O64+P64</f>
         <v>4.1000000000000005</v>
       </c>
-      <c r="V64" s="123"/>
+      <c r="V64" s="128"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6271,10 +6271,10 @@
       <c r="E65" s="54">
         <v>3</v>
       </c>
-      <c r="F65" s="115" t="s">
+      <c r="F65" s="118" t="s">
         <v>97</v>
       </c>
-      <c r="G65" s="115"/>
+      <c r="G65" s="118"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
@@ -6316,11 +6316,11 @@
         <v>12.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="124">
+      <c r="U65" s="129">
         <f t="shared" ref="U65:U70" si="23">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="124"/>
+      <c r="V65" s="129"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6348,10 +6348,10 @@
       <c r="E66" s="54">
         <v>4</v>
       </c>
-      <c r="F66" s="115" t="s">
+      <c r="F66" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="115"/>
+      <c r="G66" s="118"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
@@ -6393,11 +6393,11 @@
         <v>14.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="124">
+      <c r="U66" s="129">
         <f t="shared" si="23"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="124"/>
+      <c r="V66" s="129"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6425,10 +6425,10 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="115" t="s">
+      <c r="F67" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="G67" s="115"/>
+      <c r="G67" s="118"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
@@ -6470,11 +6470,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="124">
+      <c r="U67" s="129">
         <f t="shared" si="23"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="124"/>
+      <c r="V67" s="129"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6498,10 +6498,10 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="115" t="s">
+      <c r="F68" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="115"/>
+      <c r="G68" s="118"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
@@ -6543,11 +6543,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="124">
+      <c r="U68" s="129">
         <f t="shared" si="23"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="124"/>
+      <c r="V68" s="129"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -6571,10 +6571,10 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="115" t="s">
+      <c r="F69" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="115"/>
+      <c r="G69" s="118"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
@@ -6616,11 +6616,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="124">
+      <c r="U69" s="129">
         <f t="shared" si="23"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="124"/>
+      <c r="V69" s="129"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -6644,10 +6644,10 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="115" t="s">
+      <c r="F70" s="118" t="s">
         <v>118</v>
       </c>
-      <c r="G70" s="115"/>
+      <c r="G70" s="118"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
@@ -6689,11 +6689,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="124">
+      <c r="U70" s="129">
         <f t="shared" si="23"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="124"/>
+      <c r="V70" s="129"/>
       <c r="W70" s="25" t="s">
         <v>76</v>
       </c>
@@ -6706,12 +6706,12 @@
     <row r="71" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="72" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="73" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="O73" s="127" t="s">
+      <c r="O73" s="120" t="s">
         <v>170</v>
       </c>
-      <c r="P73" s="127"/>
-      <c r="Q73" s="127"/>
-      <c r="R73" s="127"/>
+      <c r="P73" s="120"/>
+      <c r="Q73" s="120"/>
+      <c r="R73" s="120"/>
     </row>
     <row r="74" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="35"/>
@@ -6727,31 +6727,31 @@
       <c r="E74" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="F74" s="117" t="s">
+      <c r="F74" s="130" t="s">
         <v>138</v>
       </c>
-      <c r="G74" s="117"/>
-      <c r="H74" s="117" t="s">
+      <c r="G74" s="130"/>
+      <c r="H74" s="130" t="s">
         <v>139</v>
       </c>
-      <c r="I74" s="117"/>
-      <c r="J74" s="117" t="s">
+      <c r="I74" s="130"/>
+      <c r="J74" s="130" t="s">
         <v>136</v>
       </c>
-      <c r="K74" s="117"/>
-      <c r="L74" s="117"/>
-      <c r="M74" s="117"/>
+      <c r="K74" s="130"/>
+      <c r="L74" s="130"/>
+      <c r="M74" s="130"/>
       <c r="N74" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="O74" s="117" t="s">
+      <c r="O74" s="130" t="s">
         <v>172</v>
       </c>
-      <c r="P74" s="117"/>
-      <c r="Q74" s="117" t="s">
+      <c r="P74" s="130"/>
+      <c r="Q74" s="130" t="s">
         <v>173</v>
       </c>
-      <c r="R74" s="117"/>
+      <c r="R74" s="130"/>
     </row>
     <row r="75" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="38" t="e" vm="28">
@@ -6854,16 +6854,16 @@
       <c r="L77" s="114"/>
       <c r="M77" s="114"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="132"/>
-      <c r="P77" s="132"/>
-      <c r="Q77" s="132"/>
-      <c r="R77" s="132"/>
+      <c r="O77" s="117"/>
+      <c r="P77" s="117"/>
+      <c r="Q77" s="117"/>
+      <c r="R77" s="117"/>
     </row>
     <row r="78" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="134" t="s">
+      <c r="A78" s="112" t="s">
         <v>204</v>
       </c>
-      <c r="B78" s="134" t="s">
+      <c r="B78" s="112" t="s">
         <v>203</v>
       </c>
     </row>
@@ -6885,32 +6885,32 @@
       <c r="E81" s="107" t="s">
         <v>147</v>
       </c>
-      <c r="F81" s="117" t="s">
+      <c r="F81" s="130" t="s">
         <v>142</v>
       </c>
-      <c r="G81" s="117"/>
-      <c r="H81" s="117"/>
-      <c r="I81" s="117"/>
-      <c r="J81" s="117"/>
-      <c r="K81" s="117"/>
-      <c r="L81" s="117"/>
-      <c r="M81" s="117"/>
-      <c r="N81" s="117"/>
-      <c r="O81" s="117"/>
-      <c r="P81" s="117"/>
-      <c r="Q81" s="117" t="s">
+      <c r="G81" s="130"/>
+      <c r="H81" s="130"/>
+      <c r="I81" s="130"/>
+      <c r="J81" s="130"/>
+      <c r="K81" s="130"/>
+      <c r="L81" s="130"/>
+      <c r="M81" s="130"/>
+      <c r="N81" s="130"/>
+      <c r="O81" s="130"/>
+      <c r="P81" s="130"/>
+      <c r="Q81" s="130" t="s">
         <v>157</v>
       </c>
-      <c r="R81" s="117"/>
-      <c r="S81" s="117"/>
-      <c r="T81" s="117"/>
-      <c r="U81" s="117"/>
-      <c r="V81" s="117"/>
-      <c r="W81" s="117"/>
-      <c r="X81" s="117"/>
-      <c r="Y81" s="117"/>
-      <c r="Z81" s="117"/>
-      <c r="AA81" s="117"/>
+      <c r="R81" s="130"/>
+      <c r="S81" s="130"/>
+      <c r="T81" s="130"/>
+      <c r="U81" s="130"/>
+      <c r="V81" s="130"/>
+      <c r="W81" s="130"/>
+      <c r="X81" s="130"/>
+      <c r="Y81" s="130"/>
+      <c r="Z81" s="130"/>
+      <c r="AA81" s="130"/>
     </row>
     <row r="82" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="38"/>
@@ -6926,32 +6926,32 @@
       <c r="E82" s="97">
         <v>16</v>
       </c>
-      <c r="F82" s="125" t="s">
+      <c r="F82" s="131" t="s">
         <v>153</v>
       </c>
-      <c r="G82" s="125"/>
-      <c r="H82" s="125"/>
-      <c r="I82" s="125"/>
-      <c r="J82" s="125"/>
-      <c r="K82" s="125"/>
-      <c r="L82" s="125"/>
-      <c r="M82" s="125"/>
-      <c r="N82" s="125"/>
-      <c r="O82" s="125"/>
-      <c r="P82" s="125"/>
-      <c r="Q82" s="125" t="s">
+      <c r="G82" s="131"/>
+      <c r="H82" s="131"/>
+      <c r="I82" s="131"/>
+      <c r="J82" s="131"/>
+      <c r="K82" s="131"/>
+      <c r="L82" s="131"/>
+      <c r="M82" s="131"/>
+      <c r="N82" s="131"/>
+      <c r="O82" s="131"/>
+      <c r="P82" s="131"/>
+      <c r="Q82" s="131" t="s">
         <v>158</v>
       </c>
-      <c r="R82" s="125"/>
-      <c r="S82" s="125"/>
-      <c r="T82" s="125"/>
-      <c r="U82" s="125"/>
-      <c r="V82" s="125"/>
-      <c r="W82" s="125"/>
-      <c r="X82" s="125"/>
-      <c r="Y82" s="125"/>
-      <c r="Z82" s="125"/>
-      <c r="AA82" s="125"/>
+      <c r="R82" s="131"/>
+      <c r="S82" s="131"/>
+      <c r="T82" s="131"/>
+      <c r="U82" s="131"/>
+      <c r="V82" s="131"/>
+      <c r="W82" s="131"/>
+      <c r="X82" s="131"/>
+      <c r="Y82" s="131"/>
+      <c r="Z82" s="131"/>
+      <c r="AA82" s="131"/>
     </row>
     <row r="83" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="38"/>
@@ -6967,30 +6967,30 @@
       <c r="E83" s="54">
         <v>1</v>
       </c>
-      <c r="F83" s="118" t="s">
+      <c r="F83" s="115" t="s">
         <v>155</v>
       </c>
-      <c r="G83" s="118"/>
-      <c r="H83" s="118"/>
-      <c r="I83" s="118"/>
-      <c r="J83" s="118"/>
-      <c r="K83" s="118"/>
-      <c r="L83" s="118"/>
-      <c r="M83" s="118"/>
-      <c r="N83" s="118"/>
-      <c r="O83" s="118"/>
-      <c r="P83" s="118"/>
-      <c r="Q83" s="118"/>
-      <c r="R83" s="118"/>
-      <c r="S83" s="118"/>
-      <c r="T83" s="118"/>
-      <c r="U83" s="118"/>
-      <c r="V83" s="118"/>
-      <c r="W83" s="118"/>
-      <c r="X83" s="118"/>
-      <c r="Y83" s="118"/>
-      <c r="Z83" s="118"/>
-      <c r="AA83" s="118"/>
+      <c r="G83" s="115"/>
+      <c r="H83" s="115"/>
+      <c r="I83" s="115"/>
+      <c r="J83" s="115"/>
+      <c r="K83" s="115"/>
+      <c r="L83" s="115"/>
+      <c r="M83" s="115"/>
+      <c r="N83" s="115"/>
+      <c r="O83" s="115"/>
+      <c r="P83" s="115"/>
+      <c r="Q83" s="115"/>
+      <c r="R83" s="115"/>
+      <c r="S83" s="115"/>
+      <c r="T83" s="115"/>
+      <c r="U83" s="115"/>
+      <c r="V83" s="115"/>
+      <c r="W83" s="115"/>
+      <c r="X83" s="115"/>
+      <c r="Y83" s="115"/>
+      <c r="Z83" s="115"/>
+      <c r="AA83" s="115"/>
     </row>
     <row r="84" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="38"/>
@@ -7006,30 +7006,30 @@
       <c r="E84" s="54">
         <v>1</v>
       </c>
-      <c r="F84" s="118" t="s">
+      <c r="F84" s="115" t="s">
         <v>154</v>
       </c>
-      <c r="G84" s="118"/>
-      <c r="H84" s="118"/>
-      <c r="I84" s="118"/>
-      <c r="J84" s="118"/>
-      <c r="K84" s="118"/>
-      <c r="L84" s="118"/>
-      <c r="M84" s="118"/>
-      <c r="N84" s="118"/>
-      <c r="O84" s="118"/>
-      <c r="P84" s="118"/>
-      <c r="Q84" s="118"/>
-      <c r="R84" s="118"/>
-      <c r="S84" s="118"/>
-      <c r="T84" s="118"/>
-      <c r="U84" s="118"/>
-      <c r="V84" s="118"/>
-      <c r="W84" s="118"/>
-      <c r="X84" s="118"/>
-      <c r="Y84" s="118"/>
-      <c r="Z84" s="118"/>
-      <c r="AA84" s="118"/>
+      <c r="G84" s="115"/>
+      <c r="H84" s="115"/>
+      <c r="I84" s="115"/>
+      <c r="J84" s="115"/>
+      <c r="K84" s="115"/>
+      <c r="L84" s="115"/>
+      <c r="M84" s="115"/>
+      <c r="N84" s="115"/>
+      <c r="O84" s="115"/>
+      <c r="P84" s="115"/>
+      <c r="Q84" s="115"/>
+      <c r="R84" s="115"/>
+      <c r="S84" s="115"/>
+      <c r="T84" s="115"/>
+      <c r="U84" s="115"/>
+      <c r="V84" s="115"/>
+      <c r="W84" s="115"/>
+      <c r="X84" s="115"/>
+      <c r="Y84" s="115"/>
+      <c r="Z84" s="115"/>
+      <c r="AA84" s="115"/>
     </row>
     <row r="85" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="38"/>
@@ -7045,32 +7045,32 @@
       <c r="E85" s="54">
         <v>1</v>
       </c>
-      <c r="F85" s="118" t="s">
+      <c r="F85" s="115" t="s">
         <v>156</v>
       </c>
-      <c r="G85" s="118"/>
-      <c r="H85" s="118"/>
-      <c r="I85" s="118"/>
-      <c r="J85" s="118"/>
-      <c r="K85" s="118"/>
-      <c r="L85" s="118"/>
-      <c r="M85" s="118"/>
-      <c r="N85" s="118"/>
-      <c r="O85" s="118"/>
-      <c r="P85" s="118"/>
-      <c r="Q85" s="118" t="s">
+      <c r="G85" s="115"/>
+      <c r="H85" s="115"/>
+      <c r="I85" s="115"/>
+      <c r="J85" s="115"/>
+      <c r="K85" s="115"/>
+      <c r="L85" s="115"/>
+      <c r="M85" s="115"/>
+      <c r="N85" s="115"/>
+      <c r="O85" s="115"/>
+      <c r="P85" s="115"/>
+      <c r="Q85" s="115" t="s">
         <v>159</v>
       </c>
-      <c r="R85" s="118"/>
-      <c r="S85" s="118"/>
-      <c r="T85" s="118"/>
-      <c r="U85" s="118"/>
-      <c r="V85" s="118"/>
-      <c r="W85" s="118"/>
-      <c r="X85" s="118"/>
-      <c r="Y85" s="118"/>
-      <c r="Z85" s="118"/>
-      <c r="AA85" s="118"/>
+      <c r="R85" s="115"/>
+      <c r="S85" s="115"/>
+      <c r="T85" s="115"/>
+      <c r="U85" s="115"/>
+      <c r="V85" s="115"/>
+      <c r="W85" s="115"/>
+      <c r="X85" s="115"/>
+      <c r="Y85" s="115"/>
+      <c r="Z85" s="115"/>
+      <c r="AA85" s="115"/>
     </row>
     <row r="86" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="38"/>
@@ -7078,28 +7078,28 @@
       <c r="C86" s="65"/>
       <c r="D86" s="54"/>
       <c r="E86" s="54"/>
-      <c r="F86" s="118"/>
-      <c r="G86" s="118"/>
-      <c r="H86" s="118"/>
-      <c r="I86" s="118"/>
-      <c r="J86" s="118"/>
-      <c r="K86" s="118"/>
-      <c r="L86" s="118"/>
-      <c r="M86" s="118"/>
-      <c r="N86" s="118"/>
-      <c r="O86" s="118"/>
-      <c r="P86" s="118"/>
-      <c r="Q86" s="118"/>
-      <c r="R86" s="118"/>
-      <c r="S86" s="118"/>
-      <c r="T86" s="118"/>
-      <c r="U86" s="118"/>
-      <c r="V86" s="118"/>
-      <c r="W86" s="118"/>
-      <c r="X86" s="118"/>
-      <c r="Y86" s="118"/>
-      <c r="Z86" s="118"/>
-      <c r="AA86" s="118"/>
+      <c r="F86" s="115"/>
+      <c r="G86" s="115"/>
+      <c r="H86" s="115"/>
+      <c r="I86" s="115"/>
+      <c r="J86" s="115"/>
+      <c r="K86" s="115"/>
+      <c r="L86" s="115"/>
+      <c r="M86" s="115"/>
+      <c r="N86" s="115"/>
+      <c r="O86" s="115"/>
+      <c r="P86" s="115"/>
+      <c r="Q86" s="115"/>
+      <c r="R86" s="115"/>
+      <c r="S86" s="115"/>
+      <c r="T86" s="115"/>
+      <c r="U86" s="115"/>
+      <c r="V86" s="115"/>
+      <c r="W86" s="115"/>
+      <c r="X86" s="115"/>
+      <c r="Y86" s="115"/>
+      <c r="Z86" s="115"/>
+      <c r="AA86" s="115"/>
     </row>
     <row r="87" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="38"/>
@@ -7107,28 +7107,28 @@
       <c r="C87" s="65"/>
       <c r="D87" s="54"/>
       <c r="E87" s="54"/>
-      <c r="F87" s="118"/>
-      <c r="G87" s="118"/>
-      <c r="H87" s="118"/>
-      <c r="I87" s="118"/>
-      <c r="J87" s="118"/>
-      <c r="K87" s="118"/>
-      <c r="L87" s="118"/>
-      <c r="M87" s="118"/>
-      <c r="N87" s="118"/>
-      <c r="O87" s="118"/>
-      <c r="P87" s="118"/>
-      <c r="Q87" s="118"/>
-      <c r="R87" s="118"/>
-      <c r="S87" s="118"/>
-      <c r="T87" s="118"/>
-      <c r="U87" s="118"/>
-      <c r="V87" s="118"/>
-      <c r="W87" s="118"/>
-      <c r="X87" s="118"/>
-      <c r="Y87" s="118"/>
-      <c r="Z87" s="118"/>
-      <c r="AA87" s="118"/>
+      <c r="F87" s="115"/>
+      <c r="G87" s="115"/>
+      <c r="H87" s="115"/>
+      <c r="I87" s="115"/>
+      <c r="J87" s="115"/>
+      <c r="K87" s="115"/>
+      <c r="L87" s="115"/>
+      <c r="M87" s="115"/>
+      <c r="N87" s="115"/>
+      <c r="O87" s="115"/>
+      <c r="P87" s="115"/>
+      <c r="Q87" s="115"/>
+      <c r="R87" s="115"/>
+      <c r="S87" s="115"/>
+      <c r="T87" s="115"/>
+      <c r="U87" s="115"/>
+      <c r="V87" s="115"/>
+      <c r="W87" s="115"/>
+      <c r="X87" s="115"/>
+      <c r="Y87" s="115"/>
+      <c r="Z87" s="115"/>
+      <c r="AA87" s="115"/>
     </row>
     <row r="88" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="89" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7137,24 +7137,24 @@
       <c r="B90" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="C90" s="133" t="s">
+      <c r="C90" s="119" t="s">
         <v>182</v>
       </c>
-      <c r="D90" s="133"/>
-      <c r="E90" s="133"/>
-      <c r="F90" s="133"/>
-      <c r="G90" s="133"/>
-      <c r="H90" s="133" t="s">
+      <c r="D90" s="119"/>
+      <c r="E90" s="119"/>
+      <c r="F90" s="119"/>
+      <c r="G90" s="119"/>
+      <c r="H90" s="119" t="s">
         <v>142</v>
       </c>
-      <c r="I90" s="133"/>
-      <c r="J90" s="133"/>
-      <c r="K90" s="133"/>
-      <c r="L90" s="133"/>
-      <c r="M90" s="117" t="s">
+      <c r="I90" s="119"/>
+      <c r="J90" s="119"/>
+      <c r="K90" s="119"/>
+      <c r="L90" s="119"/>
+      <c r="M90" s="130" t="s">
         <v>191</v>
       </c>
-      <c r="N90" s="117"/>
+      <c r="N90" s="130"/>
       <c r="O90" s="107"/>
     </row>
     <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -7164,24 +7164,24 @@
       <c r="B91" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C91" s="119" t="s">
+      <c r="C91" s="116" t="s">
         <v>185</v>
       </c>
-      <c r="D91" s="119"/>
-      <c r="E91" s="119"/>
-      <c r="F91" s="119"/>
-      <c r="G91" s="119"/>
-      <c r="H91" s="119" t="s">
+      <c r="D91" s="116"/>
+      <c r="E91" s="116"/>
+      <c r="F91" s="116"/>
+      <c r="G91" s="116"/>
+      <c r="H91" s="116" t="s">
         <v>187</v>
       </c>
-      <c r="I91" s="119"/>
-      <c r="J91" s="119"/>
-      <c r="K91" s="119"/>
-      <c r="L91" s="119"/>
-      <c r="M91" s="115" t="s">
+      <c r="I91" s="116"/>
+      <c r="J91" s="116"/>
+      <c r="K91" s="116"/>
+      <c r="L91" s="116"/>
+      <c r="M91" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="N91" s="115"/>
+      <c r="N91" s="118"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -7191,24 +7191,24 @@
       <c r="B92" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="C92" s="119" t="s">
+      <c r="C92" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="D92" s="119"/>
-      <c r="E92" s="119"/>
-      <c r="F92" s="119"/>
-      <c r="G92" s="119"/>
-      <c r="H92" s="119" t="s">
+      <c r="D92" s="116"/>
+      <c r="E92" s="116"/>
+      <c r="F92" s="116"/>
+      <c r="G92" s="116"/>
+      <c r="H92" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="I92" s="119"/>
-      <c r="J92" s="119"/>
-      <c r="K92" s="119"/>
-      <c r="L92" s="119"/>
-      <c r="M92" s="115" t="s">
+      <c r="I92" s="116"/>
+      <c r="J92" s="116"/>
+      <c r="K92" s="116"/>
+      <c r="L92" s="116"/>
+      <c r="M92" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="N92" s="115"/>
+      <c r="N92" s="118"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -7218,75 +7218,75 @@
       <c r="B93" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="C93" s="119" t="s">
+      <c r="C93" s="116" t="s">
         <v>189</v>
       </c>
-      <c r="D93" s="119"/>
-      <c r="E93" s="119"/>
-      <c r="F93" s="119"/>
-      <c r="G93" s="119"/>
-      <c r="H93" s="119" t="s">
+      <c r="D93" s="116"/>
+      <c r="E93" s="116"/>
+      <c r="F93" s="116"/>
+      <c r="G93" s="116"/>
+      <c r="H93" s="116" t="s">
         <v>186</v>
       </c>
-      <c r="I93" s="119"/>
-      <c r="J93" s="119"/>
-      <c r="K93" s="119"/>
-      <c r="L93" s="119"/>
-      <c r="M93" s="115" t="s">
+      <c r="I93" s="116"/>
+      <c r="J93" s="116"/>
+      <c r="K93" s="116"/>
+      <c r="L93" s="116"/>
+      <c r="M93" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="N93" s="115"/>
+      <c r="N93" s="118"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="38"/>
       <c r="B94" s="38"/>
-      <c r="C94" s="119"/>
-      <c r="D94" s="119"/>
-      <c r="E94" s="119"/>
-      <c r="F94" s="119"/>
-      <c r="G94" s="119"/>
-      <c r="H94" s="119"/>
-      <c r="I94" s="119"/>
-      <c r="J94" s="119"/>
-      <c r="K94" s="119"/>
-      <c r="L94" s="119"/>
-      <c r="M94" s="115"/>
-      <c r="N94" s="115"/>
+      <c r="C94" s="116"/>
+      <c r="D94" s="116"/>
+      <c r="E94" s="116"/>
+      <c r="F94" s="116"/>
+      <c r="G94" s="116"/>
+      <c r="H94" s="116"/>
+      <c r="I94" s="116"/>
+      <c r="J94" s="116"/>
+      <c r="K94" s="116"/>
+      <c r="L94" s="116"/>
+      <c r="M94" s="118"/>
+      <c r="N94" s="118"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="38"/>
       <c r="B95" s="38"/>
-      <c r="C95" s="119"/>
-      <c r="D95" s="119"/>
-      <c r="E95" s="119"/>
-      <c r="F95" s="119"/>
-      <c r="G95" s="119"/>
-      <c r="H95" s="119"/>
-      <c r="I95" s="119"/>
-      <c r="J95" s="119"/>
-      <c r="K95" s="119"/>
-      <c r="L95" s="119"/>
-      <c r="M95" s="115"/>
-      <c r="N95" s="115"/>
+      <c r="C95" s="116"/>
+      <c r="D95" s="116"/>
+      <c r="E95" s="116"/>
+      <c r="F95" s="116"/>
+      <c r="G95" s="116"/>
+      <c r="H95" s="116"/>
+      <c r="I95" s="116"/>
+      <c r="J95" s="116"/>
+      <c r="K95" s="116"/>
+      <c r="L95" s="116"/>
+      <c r="M95" s="118"/>
+      <c r="N95" s="118"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="38"/>
       <c r="B96" s="38"/>
-      <c r="C96" s="119"/>
-      <c r="D96" s="119"/>
-      <c r="E96" s="119"/>
-      <c r="F96" s="119"/>
-      <c r="G96" s="119"/>
-      <c r="H96" s="119"/>
-      <c r="I96" s="119"/>
-      <c r="J96" s="119"/>
-      <c r="K96" s="119"/>
-      <c r="L96" s="119"/>
-      <c r="M96" s="115"/>
-      <c r="N96" s="115"/>
+      <c r="C96" s="116"/>
+      <c r="D96" s="116"/>
+      <c r="E96" s="116"/>
+      <c r="F96" s="116"/>
+      <c r="G96" s="116"/>
+      <c r="H96" s="116"/>
+      <c r="I96" s="116"/>
+      <c r="J96" s="116"/>
+      <c r="K96" s="116"/>
+      <c r="L96" s="116"/>
+      <c r="M96" s="118"/>
+      <c r="N96" s="118"/>
       <c r="O96" s="65"/>
     </row>
     <row r="97" spans="2:2" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7298,32 +7298,42 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="Q85:AA85"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="Q77:R77"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H90:L90"/>
-    <mergeCell ref="H91:L91"/>
-    <mergeCell ref="H92:L92"/>
-    <mergeCell ref="H93:L93"/>
-    <mergeCell ref="H94:L94"/>
-    <mergeCell ref="H95:L95"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="Q83:AA83"/>
+    <mergeCell ref="Q84:AA84"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="F83:P83"/>
+    <mergeCell ref="F84:P84"/>
+    <mergeCell ref="F85:P85"/>
+    <mergeCell ref="F86:P86"/>
+    <mergeCell ref="F87:P87"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="O62:S62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="Q86:AA86"/>
+    <mergeCell ref="Q87:AA87"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="S40:T40"/>
     <mergeCell ref="F63:G63"/>
@@ -7348,14 +7358,45 @@
     <mergeCell ref="C41:E41"/>
     <mergeCell ref="C42:E42"/>
     <mergeCell ref="F41:H41"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="Q77:R77"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H90:L90"/>
+    <mergeCell ref="H91:L91"/>
+    <mergeCell ref="H92:L92"/>
+    <mergeCell ref="H93:L93"/>
+    <mergeCell ref="H94:L94"/>
+    <mergeCell ref="H95:L95"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="J77:M77"/>
+    <mergeCell ref="F81:P81"/>
+    <mergeCell ref="F82:P82"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M92:N92"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="Q81:AA81"/>
+    <mergeCell ref="Q82:AA82"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="Q85:AA85"/>
+    <mergeCell ref="C91:G91"/>
     <mergeCell ref="U63:V63"/>
     <mergeCell ref="U64:V64"/>
     <mergeCell ref="U65:V65"/>
     <mergeCell ref="U66:V66"/>
     <mergeCell ref="U69:V69"/>
     <mergeCell ref="U70:V70"/>
-    <mergeCell ref="F81:P81"/>
-    <mergeCell ref="F82:P82"/>
     <mergeCell ref="U67:V67"/>
     <mergeCell ref="U68:V68"/>
     <mergeCell ref="F76:G76"/>
@@ -7365,50 +7406,10 @@
     <mergeCell ref="J75:M75"/>
     <mergeCell ref="O73:R73"/>
     <mergeCell ref="J76:M76"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J74:M74"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M92:N92"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="F83:P83"/>
-    <mergeCell ref="F84:P84"/>
-    <mergeCell ref="F85:P85"/>
-    <mergeCell ref="F86:P86"/>
-    <mergeCell ref="F87:P87"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="O62:S62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="Q86:AA86"/>
-    <mergeCell ref="Q87:AA87"/>
-    <mergeCell ref="Q81:AA81"/>
-    <mergeCell ref="Q82:AA82"/>
-    <mergeCell ref="Q83:AA83"/>
-    <mergeCell ref="Q84:AA84"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E50:H50"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="C94:G94"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added many named skins
</commit_message>
<xml_diff>
--- a/BLACKOUT WIKI.xlsx
+++ b/BLACKOUT WIKI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\web\blackout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63DB324-BBCA-4C06-9033-A5F6635E7B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831F6514-6B70-4D93-8B29-F4A4BAFA4195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="39">
+  <futureMetadata name="XLRICHVALUE" count="46">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -327,8 +327,57 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="39"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="40"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="41"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="42"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="43"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="44"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="45"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="39">
+  <valueMetadata count="46">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -445,13 +494,34 @@
     </bk>
     <bk>
       <rc t="1" v="38"/>
+    </bk>
+    <bk>
+      <rc t="1" v="39"/>
+    </bk>
+    <bk>
+      <rc t="1" v="40"/>
+    </bk>
+    <bk>
+      <rc t="1" v="41"/>
+    </bk>
+    <bk>
+      <rc t="1" v="42"/>
+    </bk>
+    <bk>
+      <rc t="1" v="43"/>
+    </bk>
+    <bk>
+      <rc t="1" v="44"/>
+    </bk>
+    <bk>
+      <rc t="1" v="45"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="228">
   <si>
     <t>one mag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1218,10 +1288,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Name the user exactly to "VOID"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>This skin is to commemorate the game developer.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1319,6 +1385,66 @@
   </si>
   <si>
     <t>damage reduced by 40%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FROST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAEGEUK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GRADIENT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CANDY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PYTHON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JAVA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LINUX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Winter theme.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Korea!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The color of KAIST.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Christmas theme.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I like PYTHON.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Javascript has nothing to do with this…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Freaking penguins are cute.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2199,12 +2325,15 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2225,9 +2354,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2860,7 +2986,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="39">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="46">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -3017,6 +3143,34 @@
     <v>38</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>39</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>40</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>41</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>42</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>43</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>44</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>45</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -3070,6 +3224,13 @@
   <rel r:id="rId37"/>
   <rel r:id="rId38"/>
   <rel r:id="rId39"/>
+  <rel r:id="rId40"/>
+  <rel r:id="rId41"/>
+  <rel r:id="rId42"/>
+  <rel r:id="rId43"/>
+  <rel r:id="rId44"/>
+  <rel r:id="rId45"/>
+  <rel r:id="rId46"/>
 </richValueRels>
 </file>
 
@@ -3336,10 +3497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ99"/>
+  <dimension ref="A1:AJ118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44:H44"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101:G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3455,10 +3616,10 @@
         <v>26</v>
       </c>
       <c r="Y2" s="57"/>
-      <c r="Z2" s="120" t="s">
+      <c r="Z2" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="120"/>
+      <c r="AA2" s="121"/>
       <c r="AG2" s="43" t="s">
         <v>85</v>
       </c>
@@ -5751,7 +5912,7 @@
       <c r="D42" s="128"/>
       <c r="E42" s="128"/>
       <c r="F42" s="128" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G42" s="128"/>
       <c r="H42" s="128"/>
@@ -5776,23 +5937,23 @@
     </row>
     <row r="43" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B43" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>207</v>
-      </c>
       <c r="C43" s="124" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D43" s="124"/>
       <c r="E43" s="124"/>
       <c r="F43" s="124" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G43" s="124"/>
       <c r="H43" s="124"/>
       <c r="I43" s="124" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J43" s="124"/>
       <c r="K43" s="124"/>
@@ -5814,13 +5975,13 @@
     </row>
     <row r="44" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C44" s="124" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D44" s="124"/>
       <c r="E44" s="124"/>
@@ -5828,7 +5989,7 @@
       <c r="G44" s="124"/>
       <c r="H44" s="124"/>
       <c r="I44" s="124" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J44" s="124"/>
       <c r="K44" s="124"/>
@@ -5846,14 +6007,14 @@
     <row r="47" spans="1:26" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="35"/>
       <c r="B47" s="77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C47" s="127" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D47" s="127"/>
       <c r="E47" s="127" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F47" s="127"/>
       <c r="G47" s="127"/>
@@ -5866,14 +6027,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C48" s="128">
         <v>2</v>
       </c>
       <c r="D48" s="128"/>
       <c r="E48" s="128" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F48" s="128"/>
       <c r="G48" s="128"/>
@@ -5886,10 +6047,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C49" s="128" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D49" s="128"/>
       <c r="E49" s="128" t="s">
@@ -5917,7 +6078,7 @@
     <row r="52" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="53" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -6180,20 +6341,20 @@
       <c r="E63" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="F63" s="115" t="s">
+      <c r="F63" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="G63" s="115"/>
+      <c r="G63" s="116"/>
       <c r="H63" s="86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I63" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="J63" s="115" t="s">
+      <c r="J63" s="116" t="s">
         <v>98</v>
       </c>
-      <c r="K63" s="115"/>
+      <c r="K63" s="116"/>
       <c r="L63" s="86" t="s">
         <v>103</v>
       </c>
@@ -6217,10 +6378,10 @@
         <v>114</v>
       </c>
       <c r="T63" s="86"/>
-      <c r="U63" s="115" t="s">
+      <c r="U63" s="116" t="s">
         <v>118</v>
       </c>
-      <c r="V63" s="115"/>
+      <c r="V63" s="116"/>
       <c r="W63" s="86" t="s">
         <v>22</v>
       </c>
@@ -6258,11 +6419,11 @@
       <c r="I64" s="97">
         <v>0</v>
       </c>
-      <c r="J64" s="118">
+      <c r="J64" s="119">
         <f t="shared" ref="J64:J69" si="17">(C64-player_radius)*2</f>
         <v>16</v>
       </c>
-      <c r="K64" s="118"/>
+      <c r="K64" s="119"/>
       <c r="L64" s="97">
         <f>COUNTIF(H3:H35,"&gt;16")</f>
         <v>11</v>
@@ -6293,11 +6454,11 @@
         <v>10.100000000000001</v>
       </c>
       <c r="T64" s="97"/>
-      <c r="U64" s="116">
+      <c r="U64" s="117">
         <f>R64+O64+P64</f>
         <v>4.1000000000000005</v>
       </c>
-      <c r="V64" s="116"/>
+      <c r="V64" s="117"/>
       <c r="W64" s="104" t="s">
         <v>29</v>
       </c>
@@ -6325,21 +6486,21 @@
       <c r="E65" s="54">
         <v>3</v>
       </c>
-      <c r="F65" s="122" t="s">
+      <c r="F65" s="114" t="s">
         <v>96</v>
       </c>
-      <c r="G65" s="122"/>
+      <c r="G65" s="114"/>
       <c r="H65" s="54">
         <v>1</v>
       </c>
       <c r="I65" s="54">
         <v>0</v>
       </c>
-      <c r="J65" s="118">
+      <c r="J65" s="119">
         <f t="shared" si="17"/>
         <v>32</v>
       </c>
-      <c r="K65" s="118"/>
+      <c r="K65" s="119"/>
       <c r="L65" s="54">
         <f>COUNTIF(H3:H35,"&gt;32")</f>
         <v>2</v>
@@ -6370,11 +6531,11 @@
         <v>12.3</v>
       </c>
       <c r="T65" s="54"/>
-      <c r="U65" s="117">
+      <c r="U65" s="118">
         <f t="shared" ref="U65:U70" si="24">R65+O65+P65</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="V65" s="117"/>
+      <c r="V65" s="118"/>
       <c r="W65" s="28" t="s">
         <v>29</v>
       </c>
@@ -6402,21 +6563,21 @@
       <c r="E66" s="54">
         <v>4</v>
       </c>
-      <c r="F66" s="122" t="s">
+      <c r="F66" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="122"/>
+      <c r="G66" s="114"/>
       <c r="H66" s="54">
         <v>1</v>
       </c>
       <c r="I66" s="54">
         <v>11.11</v>
       </c>
-      <c r="J66" s="118">
+      <c r="J66" s="119">
         <f t="shared" si="17"/>
         <v>28</v>
       </c>
-      <c r="K66" s="118"/>
+      <c r="K66" s="119"/>
       <c r="L66" s="54">
         <f>COUNTIF(H3:H35,"&gt;28")</f>
         <v>4</v>
@@ -6447,11 +6608,11 @@
         <v>14.399999999999999</v>
       </c>
       <c r="T66" s="54"/>
-      <c r="U66" s="117">
+      <c r="U66" s="118">
         <f t="shared" si="24"/>
         <v>10.399999999999999</v>
       </c>
-      <c r="V66" s="117"/>
+      <c r="V66" s="118"/>
       <c r="W66" s="28" t="s">
         <v>29</v>
       </c>
@@ -6479,21 +6640,21 @@
       <c r="E67" s="54">
         <v>1</v>
       </c>
-      <c r="F67" s="122" t="s">
+      <c r="F67" s="114" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="122"/>
+      <c r="G67" s="114"/>
       <c r="H67" s="54">
         <v>1</v>
       </c>
       <c r="I67" s="54">
         <v>5.63</v>
       </c>
-      <c r="J67" s="118">
+      <c r="J67" s="119">
         <f t="shared" si="17"/>
         <v>48</v>
       </c>
-      <c r="K67" s="118"/>
+      <c r="K67" s="119"/>
       <c r="L67" s="54">
         <f>COUNTIF(H3:H35,"&gt;48")</f>
         <v>0</v>
@@ -6524,11 +6685,11 @@
         <v>18.700000000000003</v>
       </c>
       <c r="T67" s="54"/>
-      <c r="U67" s="117">
+      <c r="U67" s="118">
         <f t="shared" si="24"/>
         <v>17.7</v>
       </c>
-      <c r="V67" s="117"/>
+      <c r="V67" s="118"/>
       <c r="W67" s="21" t="s">
         <v>28</v>
       </c>
@@ -6552,21 +6713,21 @@
       <c r="E68" s="54">
         <v>0</v>
       </c>
-      <c r="F68" s="122" t="s">
+      <c r="F68" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="G68" s="122"/>
+      <c r="G68" s="114"/>
       <c r="H68" s="54">
         <v>1</v>
       </c>
       <c r="I68" s="54">
         <v>13.33</v>
       </c>
-      <c r="J68" s="118">
+      <c r="J68" s="119">
         <f t="shared" si="17"/>
         <v>72</v>
       </c>
-      <c r="K68" s="118"/>
+      <c r="K68" s="119"/>
       <c r="L68" s="54">
         <f>COUNTIF(H3:H35,"&gt;72")</f>
         <v>0</v>
@@ -6597,11 +6758,11 @@
         <v>17.100000000000001</v>
       </c>
       <c r="T68" s="54"/>
-      <c r="U68" s="117">
+      <c r="U68" s="118">
         <f t="shared" si="24"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="V68" s="117"/>
+      <c r="V68" s="118"/>
       <c r="W68" s="28" t="s">
         <v>29</v>
       </c>
@@ -6625,21 +6786,21 @@
       <c r="E69" s="54">
         <v>10</v>
       </c>
-      <c r="F69" s="122" t="s">
+      <c r="F69" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="122"/>
+      <c r="G69" s="114"/>
       <c r="H69" s="54">
         <v>1</v>
       </c>
       <c r="I69" s="54">
         <v>9.09</v>
       </c>
-      <c r="J69" s="118">
+      <c r="J69" s="119">
         <f t="shared" si="17"/>
         <v>20</v>
       </c>
-      <c r="K69" s="118"/>
+      <c r="K69" s="119"/>
       <c r="L69" s="54">
         <f>COUNTIF(H3:H35,"&gt;20")</f>
         <v>6</v>
@@ -6670,11 +6831,11 @@
         <v>18.8</v>
       </c>
       <c r="T69" s="54"/>
-      <c r="U69" s="117">
+      <c r="U69" s="118">
         <f t="shared" si="24"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="V69" s="117"/>
+      <c r="V69" s="118"/>
       <c r="W69" s="21" t="s">
         <v>28</v>
       </c>
@@ -6698,21 +6859,21 @@
       <c r="E70" s="54">
         <v>8</v>
       </c>
-      <c r="F70" s="122" t="s">
+      <c r="F70" s="114" t="s">
         <v>117</v>
       </c>
-      <c r="G70" s="122"/>
+      <c r="G70" s="114"/>
       <c r="H70" s="54">
         <v>1</v>
       </c>
       <c r="I70" s="54">
         <v>48</v>
       </c>
-      <c r="J70" s="118">
+      <c r="J70" s="119">
         <f t="shared" ref="J70" si="25">(C70-player_radius)*2</f>
         <v>24</v>
       </c>
-      <c r="K70" s="118"/>
+      <c r="K70" s="119"/>
       <c r="L70" s="54">
         <f>COUNTIF(H3:H35,"&gt;24")</f>
         <v>4</v>
@@ -6743,11 +6904,11 @@
         <v>25.799999999999997</v>
       </c>
       <c r="T70" s="54"/>
-      <c r="U70" s="117">
+      <c r="U70" s="118">
         <f t="shared" si="24"/>
         <v>17.799999999999997</v>
       </c>
-      <c r="V70" s="117"/>
+      <c r="V70" s="118"/>
       <c r="W70" s="25" t="s">
         <v>75</v>
       </c>
@@ -6760,12 +6921,12 @@
     <row r="71" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="72" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="73" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="O73" s="120" t="s">
+      <c r="O73" s="121" t="s">
         <v>169</v>
       </c>
-      <c r="P73" s="120"/>
-      <c r="Q73" s="120"/>
-      <c r="R73" s="120"/>
+      <c r="P73" s="121"/>
+      <c r="Q73" s="121"/>
+      <c r="R73" s="121"/>
     </row>
     <row r="74" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="35"/>
@@ -6781,31 +6942,31 @@
       <c r="E74" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="F74" s="119" t="s">
+      <c r="F74" s="120" t="s">
         <v>137</v>
       </c>
-      <c r="G74" s="119"/>
-      <c r="H74" s="119" t="s">
+      <c r="G74" s="120"/>
+      <c r="H74" s="120" t="s">
         <v>138</v>
       </c>
-      <c r="I74" s="119"/>
-      <c r="J74" s="119" t="s">
+      <c r="I74" s="120"/>
+      <c r="J74" s="120" t="s">
         <v>135</v>
       </c>
-      <c r="K74" s="119"/>
-      <c r="L74" s="119"/>
-      <c r="M74" s="119"/>
+      <c r="K74" s="120"/>
+      <c r="L74" s="120"/>
+      <c r="M74" s="120"/>
       <c r="N74" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="O74" s="119" t="s">
+      <c r="O74" s="120" t="s">
         <v>171</v>
       </c>
-      <c r="P74" s="119"/>
-      <c r="Q74" s="119" t="s">
+      <c r="P74" s="120"/>
+      <c r="Q74" s="120" t="s">
         <v>172</v>
       </c>
-      <c r="R74" s="119"/>
+      <c r="R74" s="120"/>
     </row>
     <row r="75" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="38" t="e" vm="28">
@@ -6823,21 +6984,21 @@
       <c r="E75" s="54">
         <v>18</v>
       </c>
-      <c r="F75" s="118" t="s">
+      <c r="F75" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="G75" s="118"/>
-      <c r="H75" s="118">
+      <c r="G75" s="119"/>
+      <c r="H75" s="119">
         <f>E75*frag_damage</f>
         <v>36</v>
       </c>
-      <c r="I75" s="118"/>
-      <c r="J75" s="118" t="s">
+      <c r="I75" s="119"/>
+      <c r="J75" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="K75" s="118"/>
-      <c r="L75" s="118"/>
-      <c r="M75" s="118"/>
+      <c r="K75" s="119"/>
+      <c r="L75" s="119"/>
+      <c r="M75" s="119"/>
       <c r="N75" s="78" t="e" vm="29">
         <v>#VALUE!</v>
       </c>
@@ -6866,21 +7027,21 @@
       <c r="E76" s="54">
         <v>12</v>
       </c>
-      <c r="F76" s="118" t="s">
+      <c r="F76" s="119" t="s">
         <v>127</v>
       </c>
-      <c r="G76" s="118"/>
-      <c r="H76" s="118">
+      <c r="G76" s="119"/>
+      <c r="H76" s="119">
         <f>E76*shockWave_damage</f>
         <v>180</v>
       </c>
-      <c r="I76" s="118"/>
-      <c r="J76" s="118" t="s">
+      <c r="I76" s="119"/>
+      <c r="J76" s="119" t="s">
         <v>133</v>
       </c>
-      <c r="K76" s="118"/>
-      <c r="L76" s="118"/>
-      <c r="M76" s="118"/>
+      <c r="K76" s="119"/>
+      <c r="L76" s="119"/>
+      <c r="M76" s="119"/>
       <c r="N76" s="78" t="e" vm="33">
         <v>#VALUE!</v>
       </c>
@@ -6908,17 +7069,17 @@
       <c r="L77" s="124"/>
       <c r="M77" s="124"/>
       <c r="N77" s="94"/>
-      <c r="O77" s="121"/>
-      <c r="P77" s="121"/>
-      <c r="Q77" s="121"/>
-      <c r="R77" s="121"/>
+      <c r="O77" s="122"/>
+      <c r="P77" s="122"/>
+      <c r="Q77" s="122"/>
+      <c r="R77" s="122"/>
     </row>
     <row r="78" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="112" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B78" s="112" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="1:36" ht="23.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6939,32 +7100,32 @@
       <c r="E81" s="107" t="s">
         <v>146</v>
       </c>
-      <c r="F81" s="119" t="s">
+      <c r="F81" s="120" t="s">
         <v>141</v>
       </c>
-      <c r="G81" s="119"/>
-      <c r="H81" s="119"/>
-      <c r="I81" s="119"/>
-      <c r="J81" s="119"/>
-      <c r="K81" s="119"/>
-      <c r="L81" s="119"/>
-      <c r="M81" s="119"/>
-      <c r="N81" s="119"/>
-      <c r="O81" s="119"/>
-      <c r="P81" s="119"/>
-      <c r="Q81" s="119" t="s">
+      <c r="G81" s="120"/>
+      <c r="H81" s="120"/>
+      <c r="I81" s="120"/>
+      <c r="J81" s="120"/>
+      <c r="K81" s="120"/>
+      <c r="L81" s="120"/>
+      <c r="M81" s="120"/>
+      <c r="N81" s="120"/>
+      <c r="O81" s="120"/>
+      <c r="P81" s="120"/>
+      <c r="Q81" s="120" t="s">
         <v>156</v>
       </c>
-      <c r="R81" s="119"/>
-      <c r="S81" s="119"/>
-      <c r="T81" s="119"/>
-      <c r="U81" s="119"/>
-      <c r="V81" s="119"/>
-      <c r="W81" s="119"/>
-      <c r="X81" s="119"/>
-      <c r="Y81" s="119"/>
-      <c r="Z81" s="119"/>
-      <c r="AA81" s="119"/>
+      <c r="R81" s="120"/>
+      <c r="S81" s="120"/>
+      <c r="T81" s="120"/>
+      <c r="U81" s="120"/>
+      <c r="V81" s="120"/>
+      <c r="W81" s="120"/>
+      <c r="X81" s="120"/>
+      <c r="Y81" s="120"/>
+      <c r="Z81" s="120"/>
+      <c r="AA81" s="120"/>
     </row>
     <row r="82" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="38"/>
@@ -7021,30 +7182,30 @@
       <c r="E83" s="54">
         <v>1</v>
       </c>
-      <c r="F83" s="113" t="s">
+      <c r="F83" s="115" t="s">
         <v>154</v>
       </c>
-      <c r="G83" s="113"/>
-      <c r="H83" s="113"/>
-      <c r="I83" s="113"/>
-      <c r="J83" s="113"/>
-      <c r="K83" s="113"/>
-      <c r="L83" s="113"/>
-      <c r="M83" s="113"/>
-      <c r="N83" s="113"/>
-      <c r="O83" s="113"/>
-      <c r="P83" s="113"/>
-      <c r="Q83" s="113"/>
-      <c r="R83" s="113"/>
-      <c r="S83" s="113"/>
-      <c r="T83" s="113"/>
-      <c r="U83" s="113"/>
-      <c r="V83" s="113"/>
-      <c r="W83" s="113"/>
-      <c r="X83" s="113"/>
-      <c r="Y83" s="113"/>
-      <c r="Z83" s="113"/>
-      <c r="AA83" s="113"/>
+      <c r="G83" s="115"/>
+      <c r="H83" s="115"/>
+      <c r="I83" s="115"/>
+      <c r="J83" s="115"/>
+      <c r="K83" s="115"/>
+      <c r="L83" s="115"/>
+      <c r="M83" s="115"/>
+      <c r="N83" s="115"/>
+      <c r="O83" s="115"/>
+      <c r="P83" s="115"/>
+      <c r="Q83" s="115"/>
+      <c r="R83" s="115"/>
+      <c r="S83" s="115"/>
+      <c r="T83" s="115"/>
+      <c r="U83" s="115"/>
+      <c r="V83" s="115"/>
+      <c r="W83" s="115"/>
+      <c r="X83" s="115"/>
+      <c r="Y83" s="115"/>
+      <c r="Z83" s="115"/>
+      <c r="AA83" s="115"/>
     </row>
     <row r="84" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="38"/>
@@ -7060,30 +7221,30 @@
       <c r="E84" s="54">
         <v>1</v>
       </c>
-      <c r="F84" s="113" t="s">
+      <c r="F84" s="115" t="s">
         <v>153</v>
       </c>
-      <c r="G84" s="113"/>
-      <c r="H84" s="113"/>
-      <c r="I84" s="113"/>
-      <c r="J84" s="113"/>
-      <c r="K84" s="113"/>
-      <c r="L84" s="113"/>
-      <c r="M84" s="113"/>
-      <c r="N84" s="113"/>
-      <c r="O84" s="113"/>
-      <c r="P84" s="113"/>
-      <c r="Q84" s="113"/>
-      <c r="R84" s="113"/>
-      <c r="S84" s="113"/>
-      <c r="T84" s="113"/>
-      <c r="U84" s="113"/>
-      <c r="V84" s="113"/>
-      <c r="W84" s="113"/>
-      <c r="X84" s="113"/>
-      <c r="Y84" s="113"/>
-      <c r="Z84" s="113"/>
-      <c r="AA84" s="113"/>
+      <c r="G84" s="115"/>
+      <c r="H84" s="115"/>
+      <c r="I84" s="115"/>
+      <c r="J84" s="115"/>
+      <c r="K84" s="115"/>
+      <c r="L84" s="115"/>
+      <c r="M84" s="115"/>
+      <c r="N84" s="115"/>
+      <c r="O84" s="115"/>
+      <c r="P84" s="115"/>
+      <c r="Q84" s="115"/>
+      <c r="R84" s="115"/>
+      <c r="S84" s="115"/>
+      <c r="T84" s="115"/>
+      <c r="U84" s="115"/>
+      <c r="V84" s="115"/>
+      <c r="W84" s="115"/>
+      <c r="X84" s="115"/>
+      <c r="Y84" s="115"/>
+      <c r="Z84" s="115"/>
+      <c r="AA84" s="115"/>
     </row>
     <row r="85" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="38"/>
@@ -7099,65 +7260,65 @@
       <c r="E85" s="54">
         <v>1</v>
       </c>
-      <c r="F85" s="113" t="s">
+      <c r="F85" s="115" t="s">
         <v>155</v>
       </c>
-      <c r="G85" s="113"/>
-      <c r="H85" s="113"/>
-      <c r="I85" s="113"/>
-      <c r="J85" s="113"/>
-      <c r="K85" s="113"/>
-      <c r="L85" s="113"/>
-      <c r="M85" s="113"/>
-      <c r="N85" s="113"/>
-      <c r="O85" s="113"/>
-      <c r="P85" s="113"/>
-      <c r="Q85" s="113" t="s">
+      <c r="G85" s="115"/>
+      <c r="H85" s="115"/>
+      <c r="I85" s="115"/>
+      <c r="J85" s="115"/>
+      <c r="K85" s="115"/>
+      <c r="L85" s="115"/>
+      <c r="M85" s="115"/>
+      <c r="N85" s="115"/>
+      <c r="O85" s="115"/>
+      <c r="P85" s="115"/>
+      <c r="Q85" s="115" t="s">
         <v>158</v>
       </c>
-      <c r="R85" s="113"/>
-      <c r="S85" s="113"/>
-      <c r="T85" s="113"/>
-      <c r="U85" s="113"/>
-      <c r="V85" s="113"/>
-      <c r="W85" s="113"/>
-      <c r="X85" s="113"/>
-      <c r="Y85" s="113"/>
-      <c r="Z85" s="113"/>
-      <c r="AA85" s="113"/>
+      <c r="R85" s="115"/>
+      <c r="S85" s="115"/>
+      <c r="T85" s="115"/>
+      <c r="U85" s="115"/>
+      <c r="V85" s="115"/>
+      <c r="W85" s="115"/>
+      <c r="X85" s="115"/>
+      <c r="Y85" s="115"/>
+      <c r="Z85" s="115"/>
+      <c r="AA85" s="115"/>
     </row>
     <row r="86" spans="1:27" ht="23.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C86" s="65"/>
       <c r="D86" s="54"/>
       <c r="E86" s="54"/>
-      <c r="F86" s="113"/>
-      <c r="G86" s="113"/>
-      <c r="H86" s="113"/>
-      <c r="I86" s="113"/>
-      <c r="J86" s="113"/>
-      <c r="K86" s="113"/>
-      <c r="L86" s="113"/>
-      <c r="M86" s="113"/>
-      <c r="N86" s="113"/>
-      <c r="O86" s="113"/>
-      <c r="P86" s="113"/>
-      <c r="Q86" s="113"/>
-      <c r="R86" s="113"/>
-      <c r="S86" s="113"/>
-      <c r="T86" s="113"/>
-      <c r="U86" s="113"/>
-      <c r="V86" s="113"/>
-      <c r="W86" s="113"/>
-      <c r="X86" s="113"/>
-      <c r="Y86" s="113"/>
-      <c r="Z86" s="113"/>
-      <c r="AA86" s="113"/>
+      <c r="F86" s="115"/>
+      <c r="G86" s="115"/>
+      <c r="H86" s="115"/>
+      <c r="I86" s="115"/>
+      <c r="J86" s="115"/>
+      <c r="K86" s="115"/>
+      <c r="L86" s="115"/>
+      <c r="M86" s="115"/>
+      <c r="N86" s="115"/>
+      <c r="O86" s="115"/>
+      <c r="P86" s="115"/>
+      <c r="Q86" s="115"/>
+      <c r="R86" s="115"/>
+      <c r="S86" s="115"/>
+      <c r="T86" s="115"/>
+      <c r="U86" s="115"/>
+      <c r="V86" s="115"/>
+      <c r="W86" s="115"/>
+      <c r="X86" s="115"/>
+      <c r="Y86" s="115"/>
+      <c r="Z86" s="115"/>
+      <c r="AA86" s="115"/>
     </row>
     <row r="87" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="38"/>
@@ -7165,28 +7326,28 @@
       <c r="C87" s="65"/>
       <c r="D87" s="54"/>
       <c r="E87" s="54"/>
-      <c r="F87" s="113"/>
-      <c r="G87" s="113"/>
-      <c r="H87" s="113"/>
-      <c r="I87" s="113"/>
-      <c r="J87" s="113"/>
-      <c r="K87" s="113"/>
-      <c r="L87" s="113"/>
-      <c r="M87" s="113"/>
-      <c r="N87" s="113"/>
-      <c r="O87" s="113"/>
-      <c r="P87" s="113"/>
-      <c r="Q87" s="113"/>
-      <c r="R87" s="113"/>
-      <c r="S87" s="113"/>
-      <c r="T87" s="113"/>
-      <c r="U87" s="113"/>
-      <c r="V87" s="113"/>
-      <c r="W87" s="113"/>
-      <c r="X87" s="113"/>
-      <c r="Y87" s="113"/>
-      <c r="Z87" s="113"/>
-      <c r="AA87" s="113"/>
+      <c r="F87" s="115"/>
+      <c r="G87" s="115"/>
+      <c r="H87" s="115"/>
+      <c r="I87" s="115"/>
+      <c r="J87" s="115"/>
+      <c r="K87" s="115"/>
+      <c r="L87" s="115"/>
+      <c r="M87" s="115"/>
+      <c r="N87" s="115"/>
+      <c r="O87" s="115"/>
+      <c r="P87" s="115"/>
+      <c r="Q87" s="115"/>
+      <c r="R87" s="115"/>
+      <c r="S87" s="115"/>
+      <c r="T87" s="115"/>
+      <c r="U87" s="115"/>
+      <c r="V87" s="115"/>
+      <c r="W87" s="115"/>
+      <c r="X87" s="115"/>
+      <c r="Y87" s="115"/>
+      <c r="Z87" s="115"/>
+      <c r="AA87" s="115"/>
     </row>
     <row r="88" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="89" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7209,11 +7370,14 @@
       <c r="J90" s="123"/>
       <c r="K90" s="123"/>
       <c r="L90" s="123"/>
-      <c r="M90" s="119" t="s">
-        <v>190</v>
-      </c>
-      <c r="N90" s="119"/>
+      <c r="M90" s="120" t="s">
+        <v>189</v>
+      </c>
+      <c r="N90" s="120"/>
       <c r="O90" s="107"/>
+      <c r="T90" s="58" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="91" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="38" t="e" vm="37">
@@ -7222,24 +7386,24 @@
       <c r="B91" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="C91" s="114" t="s">
+      <c r="C91" s="113" t="s">
         <v>184</v>
       </c>
-      <c r="D91" s="114"/>
-      <c r="E91" s="114"/>
-      <c r="F91" s="114"/>
-      <c r="G91" s="114"/>
-      <c r="H91" s="114" t="s">
+      <c r="D91" s="113"/>
+      <c r="E91" s="113"/>
+      <c r="F91" s="113"/>
+      <c r="G91" s="113"/>
+      <c r="H91" s="113" t="s">
         <v>186</v>
       </c>
-      <c r="I91" s="114"/>
-      <c r="J91" s="114"/>
-      <c r="K91" s="114"/>
-      <c r="L91" s="114"/>
-      <c r="M91" s="122" t="s">
-        <v>191</v>
-      </c>
-      <c r="N91" s="122"/>
+      <c r="I91" s="113"/>
+      <c r="J91" s="113"/>
+      <c r="K91" s="113"/>
+      <c r="L91" s="113"/>
+      <c r="M91" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N91" s="114"/>
       <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -7249,24 +7413,24 @@
       <c r="B92" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="C92" s="114" t="s">
+      <c r="C92" s="113" t="s">
         <v>187</v>
       </c>
-      <c r="D92" s="114"/>
-      <c r="E92" s="114"/>
-      <c r="F92" s="114"/>
-      <c r="G92" s="114"/>
-      <c r="H92" s="114" t="s">
-        <v>189</v>
-      </c>
-      <c r="I92" s="114"/>
-      <c r="J92" s="114"/>
-      <c r="K92" s="114"/>
-      <c r="L92" s="114"/>
-      <c r="M92" s="122" t="s">
-        <v>191</v>
-      </c>
-      <c r="N92" s="122"/>
+      <c r="D92" s="113"/>
+      <c r="E92" s="113"/>
+      <c r="F92" s="113"/>
+      <c r="G92" s="113"/>
+      <c r="H92" s="113" t="s">
+        <v>188</v>
+      </c>
+      <c r="I92" s="113"/>
+      <c r="J92" s="113"/>
+      <c r="K92" s="113"/>
+      <c r="L92" s="113"/>
+      <c r="M92" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N92" s="114"/>
       <c r="O92" s="65"/>
     </row>
     <row r="93" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -7276,86 +7440,518 @@
       <c r="B93" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="C93" s="114" t="s">
-        <v>188</v>
-      </c>
-      <c r="D93" s="114"/>
-      <c r="E93" s="114"/>
-      <c r="F93" s="114"/>
-      <c r="G93" s="114"/>
-      <c r="H93" s="114" t="s">
+      <c r="C93" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D93" s="113"/>
+      <c r="E93" s="113"/>
+      <c r="F93" s="113"/>
+      <c r="G93" s="113"/>
+      <c r="H93" s="113" t="s">
         <v>185</v>
       </c>
-      <c r="I93" s="114"/>
-      <c r="J93" s="114"/>
-      <c r="K93" s="114"/>
-      <c r="L93" s="114"/>
-      <c r="M93" s="122" t="s">
-        <v>191</v>
-      </c>
-      <c r="N93" s="122"/>
+      <c r="I93" s="113"/>
+      <c r="J93" s="113"/>
+      <c r="K93" s="113"/>
+      <c r="L93" s="113"/>
+      <c r="M93" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N93" s="114"/>
       <c r="O93" s="65"/>
     </row>
     <row r="94" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="38"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="114"/>
-      <c r="D94" s="114"/>
-      <c r="E94" s="114"/>
-      <c r="F94" s="114"/>
-      <c r="G94" s="114"/>
-      <c r="H94" s="114"/>
-      <c r="I94" s="114"/>
-      <c r="J94" s="114"/>
-      <c r="K94" s="114"/>
-      <c r="L94" s="114"/>
-      <c r="M94" s="122"/>
-      <c r="N94" s="122"/>
+      <c r="A94" s="38" t="e" vm="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B94" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C94" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D94" s="113"/>
+      <c r="E94" s="113"/>
+      <c r="F94" s="113"/>
+      <c r="G94" s="113"/>
+      <c r="H94" s="113" t="s">
+        <v>221</v>
+      </c>
+      <c r="I94" s="113"/>
+      <c r="J94" s="113"/>
+      <c r="K94" s="113"/>
+      <c r="L94" s="113"/>
+      <c r="M94" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N94" s="114"/>
       <c r="O94" s="65"/>
     </row>
     <row r="95" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="38"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="114"/>
-      <c r="D95" s="114"/>
-      <c r="E95" s="114"/>
-      <c r="F95" s="114"/>
-      <c r="G95" s="114"/>
-      <c r="H95" s="114"/>
-      <c r="I95" s="114"/>
-      <c r="J95" s="114"/>
-      <c r="K95" s="114"/>
-      <c r="L95" s="114"/>
-      <c r="M95" s="122"/>
-      <c r="N95" s="122"/>
+      <c r="A95" s="38" t="e" vm="41">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B95" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="C95" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D95" s="113"/>
+      <c r="E95" s="113"/>
+      <c r="F95" s="113"/>
+      <c r="G95" s="113"/>
+      <c r="H95" s="113" t="s">
+        <v>222</v>
+      </c>
+      <c r="I95" s="113"/>
+      <c r="J95" s="113"/>
+      <c r="K95" s="113"/>
+      <c r="L95" s="113"/>
+      <c r="M95" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N95" s="114"/>
       <c r="O95" s="65"/>
     </row>
     <row r="96" spans="1:27" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="38"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="114"/>
-      <c r="D96" s="114"/>
-      <c r="E96" s="114"/>
-      <c r="F96" s="114"/>
-      <c r="G96" s="114"/>
-      <c r="H96" s="114"/>
-      <c r="I96" s="114"/>
-      <c r="J96" s="114"/>
-      <c r="K96" s="114"/>
-      <c r="L96" s="114"/>
-      <c r="M96" s="122"/>
-      <c r="N96" s="122"/>
+      <c r="A96" s="38" t="e" vm="42">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B96" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="C96" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D96" s="113"/>
+      <c r="E96" s="113"/>
+      <c r="F96" s="113"/>
+      <c r="G96" s="113"/>
+      <c r="H96" s="113" t="s">
+        <v>223</v>
+      </c>
+      <c r="I96" s="113"/>
+      <c r="J96" s="113"/>
+      <c r="K96" s="113"/>
+      <c r="L96" s="113"/>
+      <c r="M96" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N96" s="114"/>
       <c r="O96" s="65"/>
     </row>
-    <row r="97" spans="2:2" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" spans="2:2" ht="24.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B99" s="58" t="s">
-        <v>201</v>
-      </c>
+    <row r="97" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A97" s="38" t="e" vm="43">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B97" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="C97" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D97" s="113"/>
+      <c r="E97" s="113"/>
+      <c r="F97" s="113"/>
+      <c r="G97" s="113"/>
+      <c r="H97" s="113" t="s">
+        <v>224</v>
+      </c>
+      <c r="I97" s="113"/>
+      <c r="J97" s="113"/>
+      <c r="K97" s="113"/>
+      <c r="L97" s="113"/>
+      <c r="M97" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N97" s="114"/>
+      <c r="O97" s="65"/>
+    </row>
+    <row r="98" spans="1:15" ht="24.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A98" s="38" t="e" vm="44">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B98" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="C98" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D98" s="113"/>
+      <c r="E98" s="113"/>
+      <c r="F98" s="113"/>
+      <c r="G98" s="113"/>
+      <c r="H98" s="113" t="s">
+        <v>225</v>
+      </c>
+      <c r="I98" s="113"/>
+      <c r="J98" s="113"/>
+      <c r="K98" s="113"/>
+      <c r="L98" s="113"/>
+      <c r="M98" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N98" s="114"/>
+      <c r="O98" s="65"/>
+    </row>
+    <row r="99" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A99" s="38" t="e" vm="45">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B99" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="C99" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D99" s="113"/>
+      <c r="E99" s="113"/>
+      <c r="F99" s="113"/>
+      <c r="G99" s="113"/>
+      <c r="H99" s="113" t="s">
+        <v>226</v>
+      </c>
+      <c r="I99" s="113"/>
+      <c r="J99" s="113"/>
+      <c r="K99" s="113"/>
+      <c r="L99" s="113"/>
+      <c r="M99" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N99" s="114"/>
+      <c r="O99" s="65"/>
+    </row>
+    <row r="100" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="38" t="e" vm="46">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B100" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="C100" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="D100" s="113"/>
+      <c r="E100" s="113"/>
+      <c r="F100" s="113"/>
+      <c r="G100" s="113"/>
+      <c r="H100" s="113" t="s">
+        <v>227</v>
+      </c>
+      <c r="I100" s="113"/>
+      <c r="J100" s="113"/>
+      <c r="K100" s="113"/>
+      <c r="L100" s="113"/>
+      <c r="M100" s="114" t="s">
+        <v>190</v>
+      </c>
+      <c r="N100" s="114"/>
+      <c r="O100" s="65"/>
+    </row>
+    <row r="101" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A101" s="38"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="113"/>
+      <c r="D101" s="113"/>
+      <c r="E101" s="113"/>
+      <c r="F101" s="113"/>
+      <c r="G101" s="113"/>
+      <c r="H101" s="113"/>
+      <c r="I101" s="113"/>
+      <c r="J101" s="113"/>
+      <c r="K101" s="113"/>
+      <c r="L101" s="113"/>
+      <c r="M101" s="114"/>
+      <c r="N101" s="114"/>
+      <c r="O101" s="65"/>
+    </row>
+    <row r="102" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A102" s="38"/>
+      <c r="B102" s="38"/>
+      <c r="H102" s="113"/>
+      <c r="I102" s="113"/>
+      <c r="J102" s="113"/>
+      <c r="K102" s="113"/>
+      <c r="L102" s="113"/>
+      <c r="M102" s="114"/>
+      <c r="N102" s="114"/>
+      <c r="O102" s="65"/>
+    </row>
+    <row r="103" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A103" s="38"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="113"/>
+      <c r="D103" s="113"/>
+      <c r="E103" s="113"/>
+      <c r="F103" s="113"/>
+      <c r="G103" s="113"/>
+      <c r="H103" s="113"/>
+      <c r="I103" s="113"/>
+      <c r="J103" s="113"/>
+      <c r="K103" s="113"/>
+      <c r="L103" s="113"/>
+      <c r="M103" s="114"/>
+      <c r="N103" s="114"/>
+      <c r="O103" s="65"/>
+    </row>
+    <row r="104" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A104" s="38"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="113"/>
+      <c r="D104" s="113"/>
+      <c r="E104" s="113"/>
+      <c r="F104" s="113"/>
+      <c r="G104" s="113"/>
+      <c r="H104" s="113"/>
+      <c r="I104" s="113"/>
+      <c r="J104" s="113"/>
+      <c r="K104" s="113"/>
+      <c r="L104" s="113"/>
+      <c r="M104" s="114"/>
+      <c r="N104" s="114"/>
+      <c r="O104" s="65"/>
+    </row>
+    <row r="105" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A105" s="38"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="113"/>
+      <c r="D105" s="113"/>
+      <c r="E105" s="113"/>
+      <c r="F105" s="113"/>
+      <c r="G105" s="113"/>
+      <c r="H105" s="113"/>
+      <c r="I105" s="113"/>
+      <c r="J105" s="113"/>
+      <c r="K105" s="113"/>
+      <c r="L105" s="113"/>
+      <c r="M105" s="114"/>
+      <c r="N105" s="114"/>
+      <c r="O105" s="65"/>
+    </row>
+    <row r="106" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A106" s="38"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="113"/>
+      <c r="D106" s="113"/>
+      <c r="E106" s="113"/>
+      <c r="F106" s="113"/>
+      <c r="G106" s="113"/>
+      <c r="H106" s="113"/>
+      <c r="I106" s="113"/>
+      <c r="J106" s="113"/>
+      <c r="K106" s="113"/>
+      <c r="L106" s="113"/>
+      <c r="M106" s="114"/>
+      <c r="N106" s="114"/>
+      <c r="O106" s="65"/>
+    </row>
+    <row r="107" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A107" s="38"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="113"/>
+      <c r="D107" s="113"/>
+      <c r="E107" s="113"/>
+      <c r="F107" s="113"/>
+      <c r="G107" s="113"/>
+      <c r="H107" s="113"/>
+      <c r="I107" s="113"/>
+      <c r="J107" s="113"/>
+      <c r="K107" s="113"/>
+      <c r="L107" s="113"/>
+      <c r="M107" s="114"/>
+      <c r="N107" s="114"/>
+      <c r="O107" s="65"/>
+    </row>
+    <row r="108" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A108" s="38"/>
+      <c r="B108" s="38"/>
+      <c r="C108" s="113"/>
+      <c r="D108" s="113"/>
+      <c r="E108" s="113"/>
+      <c r="F108" s="113"/>
+      <c r="G108" s="113"/>
+      <c r="H108" s="113"/>
+      <c r="I108" s="113"/>
+      <c r="J108" s="113"/>
+      <c r="K108" s="113"/>
+      <c r="L108" s="113"/>
+      <c r="M108" s="114"/>
+      <c r="N108" s="114"/>
+      <c r="O108" s="65"/>
+    </row>
+    <row r="109" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A109" s="38"/>
+      <c r="B109" s="38"/>
+      <c r="C109" s="113"/>
+      <c r="D109" s="113"/>
+      <c r="E109" s="113"/>
+      <c r="F109" s="113"/>
+      <c r="G109" s="113"/>
+      <c r="H109" s="113"/>
+      <c r="I109" s="113"/>
+      <c r="J109" s="113"/>
+      <c r="K109" s="113"/>
+      <c r="L109" s="113"/>
+      <c r="M109" s="114"/>
+      <c r="N109" s="114"/>
+      <c r="O109" s="65"/>
+    </row>
+    <row r="110" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A110" s="38"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="113"/>
+      <c r="D110" s="113"/>
+      <c r="E110" s="113"/>
+      <c r="F110" s="113"/>
+      <c r="G110" s="113"/>
+      <c r="H110" s="113"/>
+      <c r="I110" s="113"/>
+      <c r="J110" s="113"/>
+      <c r="K110" s="113"/>
+      <c r="L110" s="113"/>
+      <c r="M110" s="114"/>
+      <c r="N110" s="114"/>
+      <c r="O110" s="65"/>
+    </row>
+    <row r="111" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A111" s="38"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="113"/>
+      <c r="D111" s="113"/>
+      <c r="E111" s="113"/>
+      <c r="F111" s="113"/>
+      <c r="G111" s="113"/>
+      <c r="H111" s="113"/>
+      <c r="I111" s="113"/>
+      <c r="J111" s="113"/>
+      <c r="K111" s="113"/>
+      <c r="L111" s="113"/>
+      <c r="M111" s="114"/>
+      <c r="N111" s="114"/>
+      <c r="O111" s="65"/>
+    </row>
+    <row r="112" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A112" s="38"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="113"/>
+      <c r="D112" s="113"/>
+      <c r="E112" s="113"/>
+      <c r="F112" s="113"/>
+      <c r="G112" s="113"/>
+      <c r="H112" s="113"/>
+      <c r="I112" s="113"/>
+      <c r="J112" s="113"/>
+      <c r="K112" s="113"/>
+      <c r="L112" s="113"/>
+      <c r="M112" s="114"/>
+      <c r="N112" s="114"/>
+      <c r="O112" s="65"/>
+    </row>
+    <row r="113" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A113" s="38"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="113"/>
+      <c r="D113" s="113"/>
+      <c r="E113" s="113"/>
+      <c r="F113" s="113"/>
+      <c r="G113" s="113"/>
+      <c r="H113" s="113"/>
+      <c r="I113" s="113"/>
+      <c r="J113" s="113"/>
+      <c r="K113" s="113"/>
+      <c r="L113" s="113"/>
+      <c r="M113" s="114"/>
+      <c r="N113" s="114"/>
+      <c r="O113" s="65"/>
+    </row>
+    <row r="114" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A114" s="38"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="113"/>
+      <c r="D114" s="113"/>
+      <c r="E114" s="113"/>
+      <c r="F114" s="113"/>
+      <c r="G114" s="113"/>
+      <c r="H114" s="113"/>
+      <c r="I114" s="113"/>
+      <c r="J114" s="113"/>
+      <c r="K114" s="113"/>
+      <c r="L114" s="113"/>
+      <c r="M114" s="114"/>
+      <c r="N114" s="114"/>
+      <c r="O114" s="65"/>
+    </row>
+    <row r="115" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A115" s="38"/>
+      <c r="B115" s="38"/>
+      <c r="C115" s="113"/>
+      <c r="D115" s="113"/>
+      <c r="E115" s="113"/>
+      <c r="F115" s="113"/>
+      <c r="G115" s="113"/>
+      <c r="H115" s="113"/>
+      <c r="I115" s="113"/>
+      <c r="J115" s="113"/>
+      <c r="K115" s="113"/>
+      <c r="L115" s="113"/>
+      <c r="M115" s="114"/>
+      <c r="N115" s="114"/>
+      <c r="O115" s="65"/>
+    </row>
+    <row r="116" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A116" s="38"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="113"/>
+      <c r="D116" s="113"/>
+      <c r="E116" s="113"/>
+      <c r="F116" s="113"/>
+      <c r="G116" s="113"/>
+      <c r="H116" s="113"/>
+      <c r="I116" s="113"/>
+      <c r="J116" s="113"/>
+      <c r="K116" s="113"/>
+      <c r="L116" s="113"/>
+      <c r="M116" s="114"/>
+      <c r="N116" s="114"/>
+      <c r="O116" s="65"/>
+    </row>
+    <row r="117" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A117" s="38"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="113"/>
+      <c r="D117" s="113"/>
+      <c r="E117" s="113"/>
+      <c r="F117" s="113"/>
+      <c r="G117" s="113"/>
+      <c r="H117" s="113"/>
+      <c r="I117" s="113"/>
+      <c r="J117" s="113"/>
+      <c r="K117" s="113"/>
+      <c r="L117" s="113"/>
+      <c r="M117" s="114"/>
+      <c r="N117" s="114"/>
+      <c r="O117" s="65"/>
+    </row>
+    <row r="118" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A118" s="38"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="113"/>
+      <c r="D118" s="113"/>
+      <c r="E118" s="113"/>
+      <c r="F118" s="113"/>
+      <c r="G118" s="113"/>
+      <c r="H118" s="113"/>
+      <c r="I118" s="113"/>
+      <c r="J118" s="113"/>
+      <c r="K118" s="113"/>
+      <c r="L118" s="113"/>
+      <c r="M118" s="114"/>
+      <c r="N118" s="114"/>
+      <c r="O118" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="108">
+  <mergeCells count="173">
     <mergeCell ref="M96:N96"/>
     <mergeCell ref="C94:G94"/>
     <mergeCell ref="Q83:AA83"/>
@@ -7464,6 +8060,71 @@
     <mergeCell ref="J75:M75"/>
     <mergeCell ref="O73:R73"/>
     <mergeCell ref="J76:M76"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="H97:L97"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="H98:L98"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="H99:L99"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H100:L100"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="H101:L101"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="H102:L102"/>
+    <mergeCell ref="M102:N102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="M103:N103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="H104:L104"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="H105:L105"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="H106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="H107:L107"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="H108:L108"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="H109:L109"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="H110:L110"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="H111:L111"/>
+    <mergeCell ref="M111:N111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="H112:L112"/>
+    <mergeCell ref="M112:N112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H113:L113"/>
+    <mergeCell ref="M113:N113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="H114:L114"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="H118:L118"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="H115:L115"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="H116:L116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="H117:L117"/>
+    <mergeCell ref="M117:N117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>